<commit_message>
GUI changes. Variable move info added. Bugfixes and EK-specific edits to Gen3Save.
</commit_message>
<xml_diff>
--- a/data/gen3moves.xlsx
+++ b/data/gen3moves.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Projects\EKhelper\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353C26D4-C5EF-4156-A6A0-4A200A55EA08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD6BDBC-659D-465F-B7F6-5A4F4CECD2C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3171,8 +3171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G355"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
-      <selection activeCell="C176" sqref="C176"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Bugfixes and x-scissor documentation
</commit_message>
<xml_diff>
--- a/data/gen3moves.xlsx
+++ b/data/gen3moves.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Projects\EKhelper\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD6BDBC-659D-465F-B7F6-5A4F4CECD2C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEACF57C-667B-4BAA-A8FB-0F42CF19FC3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -709,9 +709,6 @@
     <t>X-Scissors</t>
   </si>
   <si>
-    <t>(!EK Move change from Fury Cutter! Includes high crit ratio!)The base power of this move doubles with each consecutive hit; however, power is capped at a maximum 160 BP and remains there for any subsequent uses. If this move misses, or if the user selects another move, base power will be reset to 10 BP on the next turn.</t>
-  </si>
-  <si>
     <t>Bug</t>
   </si>
   <si>
@@ -1865,6 +1862,9 @@
   </si>
   <si>
     <t>(! EK move change from Spark!) Has a 30% chance to paralyze the target. 1/3rd recoil damage.</t>
+  </si>
+  <si>
+    <t>Has a high crit ratio</t>
   </si>
 </sst>
 </file>
@@ -3171,8 +3171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G355"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="E113" sqref="E113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5741,19 +5741,19 @@
         <v>228</v>
       </c>
       <c r="B112" s="36" t="s">
+        <v>614</v>
+      </c>
+      <c r="C112" s="37" t="s">
         <v>229</v>
       </c>
-      <c r="C112" s="37" t="s">
-        <v>230</v>
-      </c>
       <c r="D112" s="37">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E112" s="37">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="F112" s="63">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G112" t="s">
         <v>21</v>
@@ -5761,7 +5761,7 @@
     </row>
     <row r="113" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B113" s="77" t="s">
         <v>52</v>
@@ -5784,10 +5784,10 @@
     </row>
     <row r="114" spans="1:7" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
+        <v>231</v>
+      </c>
+      <c r="B114" s="8" t="s">
         <v>232</v>
-      </c>
-      <c r="B114" s="8" t="s">
-        <v>233</v>
       </c>
       <c r="C114" s="9" t="s">
         <v>26</v>
@@ -5807,7 +5807,7 @@
     </row>
     <row r="115" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>8</v>
@@ -5830,10 +5830,10 @@
     </row>
     <row r="116" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
+        <v>234</v>
+      </c>
+      <c r="B116" s="77" t="s">
         <v>235</v>
-      </c>
-      <c r="B116" s="77" t="s">
-        <v>236</v>
       </c>
       <c r="C116" s="15" t="s">
         <v>41</v>
@@ -5853,10 +5853,10 @@
     </row>
     <row r="117" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
+        <v>236</v>
+      </c>
+      <c r="B117" s="77" t="s">
         <v>237</v>
-      </c>
-      <c r="B117" s="77" t="s">
-        <v>238</v>
       </c>
       <c r="C117" s="3" t="s">
         <v>9</v>
@@ -5876,10 +5876,10 @@
     </row>
     <row r="118" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
+        <v>238</v>
+      </c>
+      <c r="B118" s="77" t="s">
         <v>239</v>
-      </c>
-      <c r="B118" s="77" t="s">
-        <v>240</v>
       </c>
       <c r="C118" s="15" t="s">
         <v>41</v>
@@ -5899,10 +5899,10 @@
     </row>
     <row r="119" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
+        <v>240</v>
+      </c>
+      <c r="B119" s="77" t="s">
         <v>241</v>
-      </c>
-      <c r="B119" s="77" t="s">
-        <v>242</v>
       </c>
       <c r="C119" s="15" t="s">
         <v>41</v>
@@ -5922,10 +5922,10 @@
     </row>
     <row r="120" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
+        <v>242</v>
+      </c>
+      <c r="B120" s="16" t="s">
         <v>243</v>
-      </c>
-      <c r="B120" s="16" t="s">
-        <v>244</v>
       </c>
       <c r="C120" s="17" t="s">
         <v>45</v>
@@ -5945,10 +5945,10 @@
     </row>
     <row r="121" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
+        <v>244</v>
+      </c>
+      <c r="B121" s="77" t="s">
         <v>245</v>
-      </c>
-      <c r="B121" s="77" t="s">
-        <v>246</v>
       </c>
       <c r="C121" s="15" t="s">
         <v>41</v>
@@ -5957,7 +5957,7 @@
         <v>5</v>
       </c>
       <c r="E121" s="15" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F121" s="49">
         <v>0.3</v>
@@ -5968,10 +5968,10 @@
     </row>
     <row r="122" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
+        <v>247</v>
+      </c>
+      <c r="B122" s="6" t="s">
         <v>248</v>
-      </c>
-      <c r="B122" s="6" t="s">
-        <v>249</v>
       </c>
       <c r="C122" s="7" t="s">
         <v>20</v>
@@ -5991,10 +5991,10 @@
     </row>
     <row r="123" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
+        <v>249</v>
+      </c>
+      <c r="B123" s="18" t="s">
         <v>250</v>
-      </c>
-      <c r="B123" s="18" t="s">
-        <v>251</v>
       </c>
       <c r="C123" s="19" t="s">
         <v>50</v>
@@ -6014,10 +6014,10 @@
     </row>
     <row r="124" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
+        <v>251</v>
+      </c>
+      <c r="B124" s="77" t="s">
         <v>252</v>
-      </c>
-      <c r="B124" s="77" t="s">
-        <v>253</v>
       </c>
       <c r="C124" s="15" t="s">
         <v>41</v>
@@ -6037,10 +6037,10 @@
     </row>
     <row r="125" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
+        <v>253</v>
+      </c>
+      <c r="B125" s="77" t="s">
         <v>254</v>
-      </c>
-      <c r="B125" s="77" t="s">
-        <v>255</v>
       </c>
       <c r="C125" s="19" t="s">
         <v>50</v>
@@ -6060,7 +6060,7 @@
     </row>
     <row r="126" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B126" s="77" t="s">
         <v>67</v>
@@ -6083,10 +6083,10 @@
     </row>
     <row r="127" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
+        <v>256</v>
+      </c>
+      <c r="B127" s="14" t="s">
         <v>257</v>
-      </c>
-      <c r="B127" s="14" t="s">
-        <v>258</v>
       </c>
       <c r="C127" s="15" t="s">
         <v>41</v>
@@ -6106,7 +6106,7 @@
     </row>
     <row r="128" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B128" s="77" t="s">
         <v>175</v>
@@ -6129,10 +6129,10 @@
     </row>
     <row r="129" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
+        <v>259</v>
+      </c>
+      <c r="B129" s="77" t="s">
         <v>260</v>
-      </c>
-      <c r="B129" s="77" t="s">
-        <v>261</v>
       </c>
       <c r="C129" s="15" t="s">
         <v>41</v>
@@ -6152,10 +6152,10 @@
     </row>
     <row r="130" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
+        <v>261</v>
+      </c>
+      <c r="B130" s="12" t="s">
         <v>262</v>
-      </c>
-      <c r="B130" s="12" t="s">
-        <v>263</v>
       </c>
       <c r="C130" s="13" t="s">
         <v>36</v>
@@ -6175,10 +6175,10 @@
     </row>
     <row r="131" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
+        <v>263</v>
+      </c>
+      <c r="B131" s="14" t="s">
         <v>264</v>
-      </c>
-      <c r="B131" s="14" t="s">
-        <v>265</v>
       </c>
       <c r="C131" s="15" t="s">
         <v>41</v>
@@ -6198,7 +6198,7 @@
     </row>
     <row r="132" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B132" s="14" t="s">
         <v>83</v>
@@ -6221,10 +6221,10 @@
     </row>
     <row r="133" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
+        <v>266</v>
+      </c>
+      <c r="B133" s="77" t="s">
         <v>267</v>
-      </c>
-      <c r="B133" s="77" t="s">
-        <v>268</v>
       </c>
       <c r="C133" s="15" t="s">
         <v>41</v>
@@ -6244,10 +6244,10 @@
     </row>
     <row r="134" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
+        <v>268</v>
+      </c>
+      <c r="B134" s="77" t="s">
         <v>269</v>
-      </c>
-      <c r="B134" s="77" t="s">
-        <v>270</v>
       </c>
       <c r="C134" s="15" t="s">
         <v>41</v>
@@ -6267,7 +6267,7 @@
     </row>
     <row r="135" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B135" s="77" t="s">
         <v>69</v>
@@ -6290,7 +6290,7 @@
     </row>
     <row r="136" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B136" s="26" t="s">
         <v>83</v>
@@ -6313,7 +6313,7 @@
     </row>
     <row r="137" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B137" s="77" t="s">
         <v>69</v>
@@ -6336,7 +6336,7 @@
     </row>
     <row r="138" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B138" s="77" t="s">
         <v>80</v>
@@ -6359,10 +6359,10 @@
     </row>
     <row r="139" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
+        <v>274</v>
+      </c>
+      <c r="B139" s="14" t="s">
         <v>275</v>
-      </c>
-      <c r="B139" s="14" t="s">
-        <v>276</v>
       </c>
       <c r="C139" s="15" t="s">
         <v>41</v>
@@ -6382,10 +6382,10 @@
     </row>
     <row r="140" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B140" s="77" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C140" s="9" t="s">
         <v>26</v>
@@ -6405,10 +6405,10 @@
     </row>
     <row r="141" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
+        <v>277</v>
+      </c>
+      <c r="B141" s="18" t="s">
         <v>278</v>
-      </c>
-      <c r="B141" s="18" t="s">
-        <v>279</v>
       </c>
       <c r="C141" s="19" t="s">
         <v>50</v>
@@ -6428,7 +6428,7 @@
     </row>
     <row r="142" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B142" s="77" t="s">
         <v>74</v>
@@ -6451,7 +6451,7 @@
     </row>
     <row r="143" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B143" s="77" t="s">
         <v>74</v>
@@ -6474,10 +6474,10 @@
     </row>
     <row r="144" spans="1:7" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
+        <v>281</v>
+      </c>
+      <c r="B144" s="77" t="s">
         <v>282</v>
-      </c>
-      <c r="B144" s="77" t="s">
-        <v>283</v>
       </c>
       <c r="C144" s="19" t="s">
         <v>50</v>
@@ -6497,10 +6497,10 @@
     </row>
     <row r="145" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
+        <v>283</v>
+      </c>
+      <c r="B145" s="77" t="s">
         <v>284</v>
-      </c>
-      <c r="B145" s="77" t="s">
-        <v>285</v>
       </c>
       <c r="C145" s="19" t="s">
         <v>50</v>
@@ -6520,10 +6520,10 @@
     </row>
     <row r="146" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
+        <v>285</v>
+      </c>
+      <c r="B146" s="8" t="s">
         <v>286</v>
-      </c>
-      <c r="B146" s="8" t="s">
-        <v>287</v>
       </c>
       <c r="C146" s="9" t="s">
         <v>26</v>
@@ -6543,10 +6543,10 @@
     </row>
     <row r="147" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
+        <v>287</v>
+      </c>
+      <c r="B147" s="2" t="s">
         <v>288</v>
-      </c>
-      <c r="B147" s="2" t="s">
-        <v>289</v>
       </c>
       <c r="C147" s="3" t="s">
         <v>9</v>
@@ -6566,7 +6566,7 @@
     </row>
     <row r="148" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B148" s="77" t="s">
         <v>15</v>
@@ -6589,10 +6589,10 @@
     </row>
     <row r="149" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
+        <v>290</v>
+      </c>
+      <c r="B149" s="77" t="s">
         <v>291</v>
-      </c>
-      <c r="B149" s="77" t="s">
-        <v>292</v>
       </c>
       <c r="C149" s="33" t="s">
         <v>151</v>
@@ -6612,10 +6612,10 @@
     </row>
     <row r="150" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B150" s="12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C150" s="13" t="s">
         <v>36</v>
@@ -6635,7 +6635,7 @@
     </row>
     <row r="151" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B151" s="77" t="s">
         <v>23</v>
@@ -6658,7 +6658,7 @@
     </row>
     <row r="152" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B152" s="77" t="s">
         <v>211</v>
@@ -6681,10 +6681,10 @@
     </row>
     <row r="153" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
+        <v>295</v>
+      </c>
+      <c r="B153" s="20" t="s">
         <v>296</v>
-      </c>
-      <c r="B153" s="20" t="s">
-        <v>297</v>
       </c>
       <c r="C153" s="21" t="s">
         <v>58</v>
@@ -6704,7 +6704,7 @@
     </row>
     <row r="154" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B154" s="77" t="s">
         <v>23</v>
@@ -6727,13 +6727,13 @@
     </row>
     <row r="155" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B155" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C155" s="37" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D155" s="37">
         <v>24</v>
@@ -6750,10 +6750,10 @@
     </row>
     <row r="156" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
+        <v>299</v>
+      </c>
+      <c r="B156" s="2" t="s">
         <v>300</v>
-      </c>
-      <c r="B156" s="2" t="s">
-        <v>301</v>
       </c>
       <c r="C156" s="3" t="s">
         <v>9</v>
@@ -6773,10 +6773,10 @@
     </row>
     <row r="157" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
+        <v>301</v>
+      </c>
+      <c r="B157" s="77" t="s">
         <v>302</v>
-      </c>
-      <c r="B157" s="77" t="s">
-        <v>303</v>
       </c>
       <c r="C157" s="15" t="s">
         <v>41</v>
@@ -6796,7 +6796,7 @@
     </row>
     <row r="158" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B158" s="77" t="s">
         <v>78</v>
@@ -6819,10 +6819,10 @@
     </row>
     <row r="159" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
+        <v>304</v>
+      </c>
+      <c r="B159" s="8" t="s">
         <v>305</v>
-      </c>
-      <c r="B159" s="8" t="s">
-        <v>306</v>
       </c>
       <c r="C159" s="9" t="s">
         <v>26</v>
@@ -6842,10 +6842,10 @@
     </row>
     <row r="160" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
+        <v>306</v>
+      </c>
+      <c r="B160" s="14" t="s">
         <v>307</v>
-      </c>
-      <c r="B160" s="14" t="s">
-        <v>308</v>
       </c>
       <c r="C160" s="15" t="s">
         <v>41</v>
@@ -6865,10 +6865,10 @@
     </row>
     <row r="161" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B161" s="77" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C161" s="15" t="s">
         <v>41</v>
@@ -6888,10 +6888,10 @@
     </row>
     <row r="162" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
+        <v>309</v>
+      </c>
+      <c r="B162" s="77" t="s">
         <v>310</v>
-      </c>
-      <c r="B162" s="77" t="s">
-        <v>311</v>
       </c>
       <c r="C162" s="13" t="s">
         <v>36</v>
@@ -6911,10 +6911,10 @@
     </row>
     <row r="163" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
+        <v>311</v>
+      </c>
+      <c r="B163" s="77" t="s">
         <v>312</v>
-      </c>
-      <c r="B163" s="77" t="s">
-        <v>313</v>
       </c>
       <c r="C163" s="9" t="s">
         <v>26</v>
@@ -6934,7 +6934,7 @@
     </row>
     <row r="164" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B164" s="77" t="s">
         <v>188</v>
@@ -6957,10 +6957,10 @@
     </row>
     <row r="165" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
+        <v>314</v>
+      </c>
+      <c r="B165" s="8" t="s">
         <v>315</v>
-      </c>
-      <c r="B165" s="8" t="s">
-        <v>316</v>
       </c>
       <c r="C165" s="9" t="s">
         <v>26</v>
@@ -6980,7 +6980,7 @@
     </row>
     <row r="166" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B166" s="2" t="s">
         <v>19</v>
@@ -7003,10 +7003,10 @@
     </row>
     <row r="167" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
+        <v>317</v>
+      </c>
+      <c r="B167" s="24" t="s">
         <v>318</v>
-      </c>
-      <c r="B167" s="24" t="s">
-        <v>319</v>
       </c>
       <c r="C167" s="25" t="s">
         <v>81</v>
@@ -7026,7 +7026,7 @@
     </row>
     <row r="168" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B168" s="14" t="s">
         <v>76</v>
@@ -7049,10 +7049,10 @@
     </row>
     <row r="169" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B169" s="77" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C169" s="9" t="s">
         <v>26</v>
@@ -7072,7 +7072,7 @@
     </row>
     <row r="170" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B170" s="2" t="s">
         <v>8</v>
@@ -7095,7 +7095,7 @@
     </row>
     <row r="171" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B171" s="14" t="s">
         <v>83</v>
@@ -7118,7 +7118,7 @@
     </row>
     <row r="172" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B172" s="14" t="s">
         <v>83</v>
@@ -7141,13 +7141,13 @@
     </row>
     <row r="173" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B173" s="36" t="s">
         <v>83</v>
       </c>
       <c r="C173" s="37" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D173" s="37">
         <v>16</v>
@@ -7164,10 +7164,10 @@
     </row>
     <row r="174" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
+        <v>325</v>
+      </c>
+      <c r="B174" s="20" t="s">
         <v>326</v>
-      </c>
-      <c r="B174" s="20" t="s">
-        <v>327</v>
       </c>
       <c r="C174" s="21" t="s">
         <v>58</v>
@@ -7187,10 +7187,10 @@
     </row>
     <row r="175" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
+        <v>327</v>
+      </c>
+      <c r="B175" s="77" t="s">
         <v>328</v>
-      </c>
-      <c r="B175" s="77" t="s">
-        <v>329</v>
       </c>
       <c r="C175" s="33" t="s">
         <v>151</v>
@@ -7210,10 +7210,10 @@
     </row>
     <row r="176" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B176" s="77" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C176" s="33" t="s">
         <v>151</v>
@@ -7233,10 +7233,10 @@
     </row>
     <row r="177" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
+        <v>330</v>
+      </c>
+      <c r="B177" s="77" t="s">
         <v>331</v>
-      </c>
-      <c r="B177" s="77" t="s">
-        <v>332</v>
       </c>
       <c r="C177" s="33" t="s">
         <v>151</v>
@@ -7256,10 +7256,10 @@
     </row>
     <row r="178" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
+        <v>332</v>
+      </c>
+      <c r="B178" s="14" t="s">
         <v>333</v>
-      </c>
-      <c r="B178" s="14" t="s">
-        <v>334</v>
       </c>
       <c r="C178" s="15" t="s">
         <v>41</v>
@@ -7279,10 +7279,10 @@
     </row>
     <row r="179" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
+        <v>334</v>
+      </c>
+      <c r="B179" s="14" t="s">
         <v>335</v>
-      </c>
-      <c r="B179" s="14" t="s">
-        <v>336</v>
       </c>
       <c r="C179" s="15" t="s">
         <v>41</v>
@@ -7302,10 +7302,10 @@
     </row>
     <row r="180" spans="1:7" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
+        <v>336</v>
+      </c>
+      <c r="B180" s="14" t="s">
         <v>337</v>
-      </c>
-      <c r="B180" s="14" t="s">
-        <v>338</v>
       </c>
       <c r="C180" s="15" t="s">
         <v>41</v>
@@ -7325,10 +7325,10 @@
     </row>
     <row r="181" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
+        <v>338</v>
+      </c>
+      <c r="B181" s="14" t="s">
         <v>339</v>
-      </c>
-      <c r="B181" s="14" t="s">
-        <v>340</v>
       </c>
       <c r="C181" s="15" t="s">
         <v>41</v>
@@ -7348,10 +7348,10 @@
     </row>
     <row r="182" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
+        <v>340</v>
+      </c>
+      <c r="B182" s="14" t="s">
         <v>341</v>
-      </c>
-      <c r="B182" s="14" t="s">
-        <v>342</v>
       </c>
       <c r="C182" s="15" t="s">
         <v>41</v>
@@ -7371,10 +7371,10 @@
     </row>
     <row r="183" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
+        <v>342</v>
+      </c>
+      <c r="B183" s="77" t="s">
         <v>343</v>
-      </c>
-      <c r="B183" s="77" t="s">
-        <v>344</v>
       </c>
       <c r="C183" s="9" t="s">
         <v>26</v>
@@ -7394,10 +7394,10 @@
     </row>
     <row r="184" spans="1:7" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
+        <v>344</v>
+      </c>
+      <c r="B184" s="6" t="s">
         <v>345</v>
-      </c>
-      <c r="B184" s="6" t="s">
-        <v>346</v>
       </c>
       <c r="C184" s="7" t="s">
         <v>20</v>
@@ -7417,10 +7417,10 @@
     </row>
     <row r="185" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
+        <v>346</v>
+      </c>
+      <c r="B185" s="18" t="s">
         <v>347</v>
-      </c>
-      <c r="B185" s="18" t="s">
-        <v>348</v>
       </c>
       <c r="C185" s="19" t="s">
         <v>50</v>
@@ -7440,10 +7440,10 @@
     </row>
     <row r="186" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
+        <v>348</v>
+      </c>
+      <c r="B186" s="77" t="s">
         <v>349</v>
-      </c>
-      <c r="B186" s="77" t="s">
-        <v>350</v>
       </c>
       <c r="C186" s="9" t="s">
         <v>26</v>
@@ -7463,10 +7463,10 @@
     </row>
     <row r="187" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
+        <v>350</v>
+      </c>
+      <c r="B187" s="14" t="s">
         <v>351</v>
-      </c>
-      <c r="B187" s="14" t="s">
-        <v>352</v>
       </c>
       <c r="C187" s="15" t="s">
         <v>41</v>
@@ -7486,10 +7486,10 @@
     </row>
     <row r="188" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B188" s="14" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C188" s="15" t="s">
         <v>41</v>
@@ -7509,10 +7509,10 @@
     </row>
     <row r="189" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B189" s="77" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C189" s="25" t="s">
         <v>81</v>
@@ -7532,10 +7532,10 @@
     </row>
     <row r="190" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
+        <v>354</v>
+      </c>
+      <c r="B190" s="24" t="s">
         <v>355</v>
-      </c>
-      <c r="B190" s="24" t="s">
-        <v>356</v>
       </c>
       <c r="C190" s="25" t="s">
         <v>81</v>
@@ -7555,7 +7555,7 @@
     </row>
     <row r="191" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B191" s="77" t="s">
         <v>211</v>
@@ -7578,10 +7578,10 @@
     </row>
     <row r="192" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
+        <v>357</v>
+      </c>
+      <c r="B192" s="77" t="s">
         <v>358</v>
-      </c>
-      <c r="B192" s="77" t="s">
-        <v>359</v>
       </c>
       <c r="C192" s="27" t="s">
         <v>92</v>
@@ -7601,10 +7601,10 @@
     </row>
     <row r="193" spans="1:7" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
+        <v>359</v>
+      </c>
+      <c r="B193" s="14" t="s">
         <v>360</v>
-      </c>
-      <c r="B193" s="14" t="s">
-        <v>361</v>
       </c>
       <c r="C193" s="15" t="s">
         <v>41</v>
@@ -7624,7 +7624,7 @@
     </row>
     <row r="194" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B194" s="77" t="s">
         <v>67</v>
@@ -7647,10 +7647,10 @@
     </row>
     <row r="195" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
+        <v>362</v>
+      </c>
+      <c r="B195" s="16" t="s">
         <v>363</v>
-      </c>
-      <c r="B195" s="16" t="s">
-        <v>364</v>
       </c>
       <c r="C195" s="17" t="s">
         <v>45</v>
@@ -7670,10 +7670,10 @@
     </row>
     <row r="196" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
+        <v>364</v>
+      </c>
+      <c r="B196" s="77" t="s">
         <v>365</v>
-      </c>
-      <c r="B196" s="77" t="s">
-        <v>366</v>
       </c>
       <c r="C196" s="17" t="s">
         <v>45</v>
@@ -7693,10 +7693,10 @@
     </row>
     <row r="197" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
+        <v>366</v>
+      </c>
+      <c r="B197" s="77" t="s">
         <v>367</v>
-      </c>
-      <c r="B197" s="77" t="s">
-        <v>368</v>
       </c>
       <c r="C197" s="27" t="s">
         <v>92</v>
@@ -7716,7 +7716,7 @@
     </row>
     <row r="198" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B198" s="14" t="s">
         <v>223</v>
@@ -7739,10 +7739,10 @@
     </row>
     <row r="199" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
+        <v>369</v>
+      </c>
+      <c r="B199" s="34" t="s">
         <v>370</v>
-      </c>
-      <c r="B199" s="34" t="s">
-        <v>371</v>
       </c>
       <c r="C199" s="35" t="s">
         <v>159</v>
@@ -7762,10 +7762,10 @@
     </row>
     <row r="200" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
+        <v>371</v>
+      </c>
+      <c r="B200" s="77" t="s">
         <v>372</v>
-      </c>
-      <c r="B200" s="77" t="s">
-        <v>373</v>
       </c>
       <c r="C200" s="23" t="s">
         <v>70</v>
@@ -7785,10 +7785,10 @@
     </row>
     <row r="201" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
+        <v>373</v>
+      </c>
+      <c r="B201" s="14" t="s">
         <v>374</v>
-      </c>
-      <c r="B201" s="14" t="s">
-        <v>375</v>
       </c>
       <c r="C201" s="15" t="s">
         <v>41</v>
@@ -7808,10 +7808,10 @@
     </row>
     <row r="202" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
+        <v>375</v>
+      </c>
+      <c r="B202" s="77" t="s">
         <v>376</v>
-      </c>
-      <c r="B202" s="77" t="s">
-        <v>377</v>
       </c>
       <c r="C202" s="15" t="s">
         <v>41</v>
@@ -7831,7 +7831,7 @@
     </row>
     <row r="203" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B203" s="6" t="s">
         <v>83</v>
@@ -7854,10 +7854,10 @@
     </row>
     <row r="204" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
+        <v>378</v>
+      </c>
+      <c r="B204" s="77" t="s">
         <v>379</v>
-      </c>
-      <c r="B204" s="77" t="s">
-        <v>380</v>
       </c>
       <c r="C204" s="15" t="s">
         <v>41</v>
@@ -7877,10 +7877,10 @@
     </row>
     <row r="205" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
+        <v>380</v>
+      </c>
+      <c r="B205" s="2" t="s">
         <v>381</v>
-      </c>
-      <c r="B205" s="2" t="s">
-        <v>382</v>
       </c>
       <c r="C205" s="3" t="s">
         <v>9</v>
@@ -7900,13 +7900,13 @@
     </row>
     <row r="206" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B206" s="77" t="s">
         <v>52</v>
       </c>
       <c r="C206" s="37" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D206" s="37">
         <v>20</v>
@@ -7923,10 +7923,10 @@
     </row>
     <row r="207" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
+        <v>383</v>
+      </c>
+      <c r="B207" s="4" t="s">
         <v>384</v>
-      </c>
-      <c r="B207" s="4" t="s">
-        <v>385</v>
       </c>
       <c r="C207" s="5" t="s">
         <v>13</v>
@@ -7946,10 +7946,10 @@
     </row>
     <row r="208" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
+        <v>385</v>
+      </c>
+      <c r="B208" s="77" t="s">
         <v>386</v>
-      </c>
-      <c r="B208" s="77" t="s">
-        <v>387</v>
       </c>
       <c r="C208" s="5" t="s">
         <v>13</v>
@@ -7969,10 +7969,10 @@
     </row>
     <row r="209" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
+        <v>387</v>
+      </c>
+      <c r="B209" s="77" t="s">
         <v>388</v>
-      </c>
-      <c r="B209" s="77" t="s">
-        <v>389</v>
       </c>
       <c r="C209" s="5" t="s">
         <v>13</v>
@@ -7992,10 +7992,10 @@
     </row>
     <row r="210" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
+        <v>389</v>
+      </c>
+      <c r="B210" s="4" t="s">
         <v>390</v>
-      </c>
-      <c r="B210" s="4" t="s">
-        <v>391</v>
       </c>
       <c r="C210" s="5" t="s">
         <v>13</v>
@@ -8015,10 +8015,10 @@
     </row>
     <row r="211" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B211" s="77" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C211" s="5" t="s">
         <v>13</v>
@@ -8038,7 +8038,7 @@
     </row>
     <row r="212" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B212" s="14" t="s">
         <v>83</v>
@@ -8061,7 +8061,7 @@
     </row>
     <row r="213" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B213" s="77" t="s">
         <v>74</v>
@@ -8084,10 +8084,10 @@
     </row>
     <row r="214" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
+        <v>394</v>
+      </c>
+      <c r="B214" s="77" t="s">
         <v>395</v>
-      </c>
-      <c r="B214" s="77" t="s">
-        <v>396</v>
       </c>
       <c r="C214" s="15" t="s">
         <v>41</v>
@@ -8107,7 +8107,7 @@
     </row>
     <row r="215" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B215" s="14" t="s">
         <v>140</v>
@@ -8130,7 +8130,7 @@
     </row>
     <row r="216" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B216" s="77" t="s">
         <v>112</v>
@@ -8153,10 +8153,10 @@
     </row>
     <row r="217" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
+        <v>398</v>
+      </c>
+      <c r="B217" s="77" t="s">
         <v>399</v>
-      </c>
-      <c r="B217" s="77" t="s">
-        <v>400</v>
       </c>
       <c r="C217" s="15" t="s">
         <v>41</v>
@@ -8179,7 +8179,7 @@
         <v>26</v>
       </c>
       <c r="B218" s="77" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C218" s="9" t="s">
         <v>26</v>
@@ -8199,10 +8199,10 @@
     </row>
     <row r="219" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
+        <v>401</v>
+      </c>
+      <c r="B219" s="77" t="s">
         <v>402</v>
-      </c>
-      <c r="B219" s="77" t="s">
-        <v>403</v>
       </c>
       <c r="C219" s="9" t="s">
         <v>26</v>
@@ -8222,10 +8222,10 @@
     </row>
     <row r="220" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B220" s="8" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C220" s="9" t="s">
         <v>26</v>
@@ -8245,10 +8245,10 @@
     </row>
     <row r="221" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
+        <v>404</v>
+      </c>
+      <c r="B221" s="77" t="s">
         <v>405</v>
-      </c>
-      <c r="B221" s="77" t="s">
-        <v>406</v>
       </c>
       <c r="C221" s="21" t="s">
         <v>58</v>
@@ -8268,7 +8268,7 @@
     </row>
     <row r="222" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B222" s="77" t="s">
         <v>188</v>
@@ -8291,10 +8291,10 @@
     </row>
     <row r="223" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
+        <v>407</v>
+      </c>
+      <c r="B223" s="77" t="s">
         <v>408</v>
-      </c>
-      <c r="B223" s="77" t="s">
-        <v>409</v>
       </c>
       <c r="C223" s="15" t="s">
         <v>41</v>
@@ -8314,10 +8314,10 @@
     </row>
     <row r="224" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
+        <v>409</v>
+      </c>
+      <c r="B224" s="26" t="s">
         <v>410</v>
-      </c>
-      <c r="B224" s="26" t="s">
-        <v>411</v>
       </c>
       <c r="C224" s="27" t="s">
         <v>92</v>
@@ -8337,10 +8337,10 @@
     </row>
     <row r="225" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
+        <v>411</v>
+      </c>
+      <c r="B225" s="14" t="s">
         <v>412</v>
-      </c>
-      <c r="B225" s="14" t="s">
-        <v>413</v>
       </c>
       <c r="C225" s="15" t="s">
         <v>41</v>
@@ -8360,7 +8360,7 @@
     </row>
     <row r="226" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B226" s="77" t="s">
         <v>23</v>
@@ -8383,10 +8383,10 @@
     </row>
     <row r="227" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
+        <v>414</v>
+      </c>
+      <c r="B227" s="14" t="s">
         <v>415</v>
-      </c>
-      <c r="B227" s="14" t="s">
-        <v>416</v>
       </c>
       <c r="C227" s="15" t="s">
         <v>41</v>
@@ -8406,10 +8406,10 @@
     </row>
     <row r="228" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B228" s="14" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C228" s="15" t="s">
         <v>41</v>
@@ -8429,10 +8429,10 @@
     </row>
     <row r="229" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
+        <v>417</v>
+      </c>
+      <c r="B229" s="14" t="s">
         <v>418</v>
-      </c>
-      <c r="B229" s="14" t="s">
-        <v>419</v>
       </c>
       <c r="C229" s="15" t="s">
         <v>41</v>
@@ -8452,10 +8452,10 @@
     </row>
     <row r="230" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
+        <v>419</v>
+      </c>
+      <c r="B230" s="8" t="s">
         <v>420</v>
-      </c>
-      <c r="B230" s="8" t="s">
-        <v>421</v>
       </c>
       <c r="C230" s="9" t="s">
         <v>26</v>
@@ -8475,10 +8475,10 @@
     </row>
     <row r="231" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
+        <v>421</v>
+      </c>
+      <c r="B231" s="14" t="s">
         <v>422</v>
-      </c>
-      <c r="B231" s="14" t="s">
-        <v>423</v>
       </c>
       <c r="C231" s="15" t="s">
         <v>41</v>
@@ -8498,10 +8498,10 @@
     </row>
     <row r="232" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
+        <v>423</v>
+      </c>
+      <c r="B232" s="8" t="s">
         <v>424</v>
-      </c>
-      <c r="B232" s="8" t="s">
-        <v>425</v>
       </c>
       <c r="C232" s="9" t="s">
         <v>26</v>
@@ -8521,10 +8521,10 @@
     </row>
     <row r="233" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
+        <v>425</v>
+      </c>
+      <c r="B233" s="77" t="s">
         <v>426</v>
-      </c>
-      <c r="B233" s="77" t="s">
-        <v>427</v>
       </c>
       <c r="C233" s="15" t="s">
         <v>41</v>
@@ -8544,10 +8544,10 @@
     </row>
     <row r="234" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
+        <v>427</v>
+      </c>
+      <c r="B234" s="12" t="s">
         <v>428</v>
-      </c>
-      <c r="B234" s="12" t="s">
-        <v>429</v>
       </c>
       <c r="C234" s="13" t="s">
         <v>36</v>
@@ -8567,7 +8567,7 @@
     </row>
     <row r="235" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B235" s="77" t="s">
         <v>205</v>
@@ -8590,10 +8590,10 @@
     </row>
     <row r="236" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
+        <v>430</v>
+      </c>
+      <c r="B236" s="14" t="s">
         <v>431</v>
-      </c>
-      <c r="B236" s="14" t="s">
-        <v>432</v>
       </c>
       <c r="C236" s="15" t="s">
         <v>41</v>
@@ -8613,7 +8613,7 @@
     </row>
     <row r="237" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B237" s="77" t="s">
         <v>52</v>
@@ -8636,7 +8636,7 @@
     </row>
     <row r="238" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B238" s="77" t="s">
         <v>67</v>
@@ -8659,7 +8659,7 @@
     </row>
     <row r="239" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B239" s="77" t="s">
         <v>131</v>
@@ -8682,7 +8682,7 @@
     </row>
     <row r="240" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B240" s="10" t="s">
         <v>83</v>
@@ -8705,10 +8705,10 @@
     </row>
     <row r="241" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B241" s="77" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C241" s="11" t="s">
         <v>33</v>
@@ -8728,10 +8728,10 @@
     </row>
     <row r="242" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
+        <v>437</v>
+      </c>
+      <c r="B242" s="77" t="s">
         <v>438</v>
-      </c>
-      <c r="B242" s="77" t="s">
-        <v>439</v>
       </c>
       <c r="C242" s="9" t="s">
         <v>26</v>
@@ -8751,7 +8751,7 @@
     </row>
     <row r="243" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B243" s="77" t="s">
         <v>67</v>
@@ -8774,10 +8774,10 @@
     </row>
     <row r="244" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B244" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C244" s="11" t="s">
         <v>33</v>
@@ -8797,10 +8797,10 @@
     </row>
     <row r="245" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
+        <v>441</v>
+      </c>
+      <c r="B245" s="22" t="s">
         <v>442</v>
-      </c>
-      <c r="B245" s="22" t="s">
-        <v>443</v>
       </c>
       <c r="C245" s="23" t="s">
         <v>70</v>
@@ -8820,10 +8820,10 @@
     </row>
     <row r="246" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
+        <v>443</v>
+      </c>
+      <c r="B246" s="77" t="s">
         <v>444</v>
-      </c>
-      <c r="B246" s="77" t="s">
-        <v>445</v>
       </c>
       <c r="C246" s="15" t="s">
         <v>41</v>
@@ -8843,7 +8843,7 @@
     </row>
     <row r="247" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B247" s="24" t="s">
         <v>65</v>
@@ -8866,7 +8866,7 @@
     </row>
     <row r="248" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B248" s="77" t="s">
         <v>211</v>
@@ -8889,10 +8889,10 @@
     </row>
     <row r="249" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
+        <v>447</v>
+      </c>
+      <c r="B249" s="10" t="s">
         <v>448</v>
-      </c>
-      <c r="B249" s="10" t="s">
-        <v>449</v>
       </c>
       <c r="C249" s="11" t="s">
         <v>33</v>
@@ -8912,7 +8912,7 @@
     </row>
     <row r="250" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B250" s="77" t="s">
         <v>121</v>
@@ -8935,7 +8935,7 @@
     </row>
     <row r="251" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B251" s="14" t="s">
         <v>83</v>
@@ -8958,10 +8958,10 @@
     </row>
     <row r="252" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
+        <v>451</v>
+      </c>
+      <c r="B252" s="77" t="s">
         <v>452</v>
-      </c>
-      <c r="B252" s="77" t="s">
-        <v>453</v>
       </c>
       <c r="C252" s="15" t="s">
         <v>41</v>
@@ -8981,10 +8981,10 @@
     </row>
     <row r="253" spans="1:7" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
+        <v>453</v>
+      </c>
+      <c r="B253" s="14" t="s">
         <v>454</v>
-      </c>
-      <c r="B253" s="14" t="s">
-        <v>455</v>
       </c>
       <c r="C253" s="15" t="s">
         <v>41</v>
@@ -9004,10 +9004,10 @@
     </row>
     <row r="254" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B254" s="12" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C254" s="13" t="s">
         <v>36</v>
@@ -9027,7 +9027,7 @@
     </row>
     <row r="255" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B255" s="77" t="s">
         <v>185</v>
@@ -9050,7 +9050,7 @@
     </row>
     <row r="256" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B256" s="77" t="s">
         <v>129</v>
@@ -9073,7 +9073,7 @@
     </row>
     <row r="257" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B257" s="16" t="s">
         <v>19</v>
@@ -9096,10 +9096,10 @@
     </row>
     <row r="258" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B258" s="77" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C258" s="15" t="s">
         <v>41</v>
@@ -9119,10 +9119,10 @@
     </row>
     <row r="259" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B259" s="77" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C259" s="19" t="s">
         <v>50</v>
@@ -9131,7 +9131,7 @@
         <v>5</v>
       </c>
       <c r="E259" s="19" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F259" s="50">
         <v>0.3</v>
@@ -9142,7 +9142,7 @@
     </row>
     <row r="260" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B260" s="28" t="s">
         <v>19</v>
@@ -9165,13 +9165,13 @@
     </row>
     <row r="261" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B261" s="77" t="s">
         <v>112</v>
       </c>
       <c r="C261" s="37" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D261" s="37">
         <v>24</v>
@@ -9188,13 +9188,13 @@
     </row>
     <row r="262" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B262" s="77" t="s">
         <v>32</v>
       </c>
       <c r="C262" s="37" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D262" s="37">
         <v>5</v>
@@ -9211,10 +9211,10 @@
     </row>
     <row r="263" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B263" s="77" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C263" s="15" t="s">
         <v>41</v>
@@ -9234,10 +9234,10 @@
     </row>
     <row r="264" spans="1:7" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
+        <v>465</v>
+      </c>
+      <c r="B264" s="14" t="s">
         <v>466</v>
-      </c>
-      <c r="B264" s="14" t="s">
-        <v>467</v>
       </c>
       <c r="C264" s="15" t="s">
         <v>41</v>
@@ -9257,10 +9257,10 @@
     </row>
     <row r="265" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
+        <v>467</v>
+      </c>
+      <c r="B265" s="77" t="s">
         <v>468</v>
-      </c>
-      <c r="B265" s="77" t="s">
-        <v>469</v>
       </c>
       <c r="C265" s="9" t="s">
         <v>26</v>
@@ -9280,10 +9280,10 @@
     </row>
     <row r="266" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
+        <v>469</v>
+      </c>
+      <c r="B266" s="14" t="s">
         <v>470</v>
-      </c>
-      <c r="B266" s="14" t="s">
-        <v>471</v>
       </c>
       <c r="C266" s="15" t="s">
         <v>41</v>
@@ -9303,10 +9303,10 @@
     </row>
     <row r="267" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
+        <v>471</v>
+      </c>
+      <c r="B267" s="6" t="s">
         <v>472</v>
-      </c>
-      <c r="B267" s="6" t="s">
-        <v>473</v>
       </c>
       <c r="C267" s="7" t="s">
         <v>20</v>
@@ -9326,10 +9326,10 @@
     </row>
     <row r="268" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
+        <v>473</v>
+      </c>
+      <c r="B268" s="12" t="s">
         <v>474</v>
-      </c>
-      <c r="B268" s="12" t="s">
-        <v>475</v>
       </c>
       <c r="C268" s="13" t="s">
         <v>36</v>
@@ -9349,10 +9349,10 @@
     </row>
     <row r="269" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B269" s="14" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C269" s="15" t="s">
         <v>41</v>
@@ -9372,7 +9372,7 @@
     </row>
     <row r="270" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B270" s="14" t="s">
         <v>83</v>
@@ -9395,7 +9395,7 @@
     </row>
     <row r="271" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B271" s="77" t="s">
         <v>23</v>
@@ -9418,10 +9418,10 @@
     </row>
     <row r="272" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B272" s="77" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C272" s="3" t="s">
         <v>9</v>
@@ -9441,10 +9441,10 @@
     </row>
     <row r="273" spans="1:7" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
+        <v>479</v>
+      </c>
+      <c r="B273" s="14" t="s">
         <v>480</v>
-      </c>
-      <c r="B273" s="14" t="s">
-        <v>481</v>
       </c>
       <c r="C273" s="15" t="s">
         <v>41</v>
@@ -9464,10 +9464,10 @@
     </row>
     <row r="274" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
+        <v>481</v>
+      </c>
+      <c r="B274" s="77" t="s">
         <v>482</v>
-      </c>
-      <c r="B274" s="77" t="s">
-        <v>483</v>
       </c>
       <c r="C274" s="5" t="s">
         <v>13</v>
@@ -9487,10 +9487,10 @@
     </row>
     <row r="275" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B275" s="77" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C275" s="5" t="s">
         <v>13</v>
@@ -9510,10 +9510,10 @@
     </row>
     <row r="276" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
+        <v>484</v>
+      </c>
+      <c r="B276" s="77" t="s">
         <v>485</v>
-      </c>
-      <c r="B276" s="77" t="s">
-        <v>486</v>
       </c>
       <c r="C276" s="15" t="s">
         <v>41</v>
@@ -9533,10 +9533,10 @@
     </row>
     <row r="277" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
+        <v>486</v>
+      </c>
+      <c r="B277" s="77" t="s">
         <v>487</v>
-      </c>
-      <c r="B277" s="77" t="s">
-        <v>488</v>
       </c>
       <c r="C277" s="5" t="s">
         <v>13</v>
@@ -9556,7 +9556,7 @@
     </row>
     <row r="278" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B278" s="77" t="s">
         <v>211</v>
@@ -9579,10 +9579,10 @@
     </row>
     <row r="279" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
+        <v>489</v>
+      </c>
+      <c r="B279" s="20" t="s">
         <v>490</v>
-      </c>
-      <c r="B279" s="20" t="s">
-        <v>491</v>
       </c>
       <c r="C279" s="21" t="s">
         <v>58</v>
@@ -9602,10 +9602,10 @@
     </row>
     <row r="280" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
+        <v>491</v>
+      </c>
+      <c r="B280" s="77" t="s">
         <v>492</v>
-      </c>
-      <c r="B280" s="77" t="s">
-        <v>493</v>
       </c>
       <c r="C280" s="15" t="s">
         <v>41</v>
@@ -9625,10 +9625,10 @@
     </row>
     <row r="281" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B281" s="14" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C281" s="15" t="s">
         <v>41</v>
@@ -9648,10 +9648,10 @@
     </row>
     <row r="282" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
+        <v>494</v>
+      </c>
+      <c r="B282" s="2" t="s">
         <v>495</v>
-      </c>
-      <c r="B282" s="2" t="s">
-        <v>496</v>
       </c>
       <c r="C282" s="3" t="s">
         <v>9</v>
@@ -9671,10 +9671,10 @@
     </row>
     <row r="283" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
+        <v>496</v>
+      </c>
+      <c r="B283" s="14" t="s">
         <v>497</v>
-      </c>
-      <c r="B283" s="14" t="s">
-        <v>498</v>
       </c>
       <c r="C283" s="15" t="s">
         <v>41</v>
@@ -9694,10 +9694,10 @@
     </row>
     <row r="284" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B284" s="77" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C284" s="29" t="s">
         <v>104</v>
@@ -9717,13 +9717,13 @@
     </row>
     <row r="285" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B285" s="36" t="s">
         <v>76</v>
       </c>
       <c r="C285" s="37" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D285" s="37">
         <v>10</v>
@@ -9740,7 +9740,7 @@
     </row>
     <row r="286" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B286" s="77" t="s">
         <v>52</v>
@@ -9763,10 +9763,10 @@
     </row>
     <row r="287" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
+        <v>501</v>
+      </c>
+      <c r="B287" s="24" t="s">
         <v>502</v>
-      </c>
-      <c r="B287" s="24" t="s">
-        <v>503</v>
       </c>
       <c r="C287" s="25" t="s">
         <v>81</v>
@@ -9786,7 +9786,7 @@
     </row>
     <row r="288" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B288" s="14" t="s">
         <v>83</v>
@@ -9809,10 +9809,10 @@
     </row>
     <row r="289" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
+        <v>504</v>
+      </c>
+      <c r="B289" s="77" t="s">
         <v>505</v>
-      </c>
-      <c r="B289" s="77" t="s">
-        <v>506</v>
       </c>
       <c r="C289" s="17" t="s">
         <v>45</v>
@@ -9832,10 +9832,10 @@
     </row>
     <row r="290" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
+        <v>506</v>
+      </c>
+      <c r="B290" s="14" t="s">
         <v>507</v>
-      </c>
-      <c r="B290" s="14" t="s">
-        <v>508</v>
       </c>
       <c r="C290" s="15" t="s">
         <v>41</v>
@@ -9855,10 +9855,10 @@
     </row>
     <row r="291" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B291" s="77" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C291" s="3" t="s">
         <v>9</v>
@@ -9878,10 +9878,10 @@
     </row>
     <row r="292" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
+        <v>509</v>
+      </c>
+      <c r="B292" s="77" t="s">
         <v>510</v>
-      </c>
-      <c r="B292" s="77" t="s">
-        <v>511</v>
       </c>
       <c r="C292" s="33" t="s">
         <v>151</v>
@@ -9901,10 +9901,10 @@
     </row>
     <row r="293" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
+        <v>511</v>
+      </c>
+      <c r="B293" s="14" t="s">
         <v>512</v>
-      </c>
-      <c r="B293" s="14" t="s">
-        <v>513</v>
       </c>
       <c r="C293" s="15" t="s">
         <v>41</v>
@@ -9924,10 +9924,10 @@
     </row>
     <row r="294" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
+        <v>513</v>
+      </c>
+      <c r="B294" s="14" t="s">
         <v>514</v>
-      </c>
-      <c r="B294" s="14" t="s">
-        <v>515</v>
       </c>
       <c r="C294" s="15" t="s">
         <v>41</v>
@@ -9947,7 +9947,7 @@
     </row>
     <row r="295" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B295" s="14" t="s">
         <v>83</v>
@@ -9970,13 +9970,13 @@
     </row>
     <row r="296" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B296" s="77" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C296" s="37" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D296" s="37">
         <v>5</v>
@@ -9993,10 +9993,10 @@
     </row>
     <row r="297" spans="1:7" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
+        <v>517</v>
+      </c>
+      <c r="B297" s="77" t="s">
         <v>518</v>
-      </c>
-      <c r="B297" s="77" t="s">
-        <v>519</v>
       </c>
       <c r="C297" s="38" t="s">
         <v>41</v>
@@ -10016,10 +10016,10 @@
     </row>
     <row r="298" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B298" s="77" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C298" s="3" t="s">
         <v>9</v>
@@ -10039,10 +10039,10 @@
     </row>
     <row r="299" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
+        <v>520</v>
+      </c>
+      <c r="B299" s="12" t="s">
         <v>521</v>
-      </c>
-      <c r="B299" s="12" t="s">
-        <v>522</v>
       </c>
       <c r="C299" s="13" t="s">
         <v>36</v>
@@ -10062,10 +10062,10 @@
     </row>
     <row r="300" spans="1:7" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
+        <v>522</v>
+      </c>
+      <c r="B300" s="14" t="s">
         <v>523</v>
-      </c>
-      <c r="B300" s="14" t="s">
-        <v>524</v>
       </c>
       <c r="C300" s="15" t="s">
         <v>41</v>
@@ -10085,10 +10085,10 @@
     </row>
     <row r="301" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
+        <v>524</v>
+      </c>
+      <c r="B301" s="22" t="s">
         <v>525</v>
-      </c>
-      <c r="B301" s="22" t="s">
-        <v>526</v>
       </c>
       <c r="C301" s="23" t="s">
         <v>70</v>
@@ -10108,10 +10108,10 @@
     </row>
     <row r="302" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
+        <v>526</v>
+      </c>
+      <c r="B302" s="77" t="s">
         <v>527</v>
-      </c>
-      <c r="B302" s="77" t="s">
-        <v>528</v>
       </c>
       <c r="C302" s="21" t="s">
         <v>58</v>
@@ -10120,7 +10120,7 @@
         <v>16</v>
       </c>
       <c r="E302" s="21" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="F302" s="51">
         <v>1</v>
@@ -10131,10 +10131,10 @@
     </row>
     <row r="303" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
+        <v>529</v>
+      </c>
+      <c r="B303" s="77" t="s">
         <v>530</v>
-      </c>
-      <c r="B303" s="77" t="s">
-        <v>531</v>
       </c>
       <c r="C303" s="13" t="s">
         <v>36</v>
@@ -10154,7 +10154,7 @@
     </row>
     <row r="304" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B304" s="77" t="s">
         <v>110</v>
@@ -10177,10 +10177,10 @@
     </row>
     <row r="305" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
+        <v>532</v>
+      </c>
+      <c r="B305" s="77" t="s">
         <v>533</v>
-      </c>
-      <c r="B305" s="77" t="s">
-        <v>534</v>
       </c>
       <c r="C305" s="27" t="s">
         <v>92</v>
@@ -10200,10 +10200,10 @@
     </row>
     <row r="306" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
+        <v>534</v>
+      </c>
+      <c r="B306" s="14" t="s">
         <v>535</v>
-      </c>
-      <c r="B306" s="14" t="s">
-        <v>536</v>
       </c>
       <c r="C306" s="15" t="s">
         <v>41</v>
@@ -10223,10 +10223,10 @@
     </row>
     <row r="307" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B307" s="77" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C307" s="15" t="s">
         <v>41</v>
@@ -10246,7 +10246,7 @@
     </row>
     <row r="308" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B308" s="77" t="s">
         <v>110</v>
@@ -10269,10 +10269,10 @@
     </row>
     <row r="309" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
+        <v>538</v>
+      </c>
+      <c r="B309" s="77" t="s">
         <v>539</v>
-      </c>
-      <c r="B309" s="77" t="s">
-        <v>540</v>
       </c>
       <c r="C309" s="15" t="s">
         <v>41</v>
@@ -10292,7 +10292,7 @@
     </row>
     <row r="310" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B310" s="14" t="s">
         <v>19</v>
@@ -10315,10 +10315,10 @@
     </row>
     <row r="311" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
+        <v>541</v>
+      </c>
+      <c r="B311" s="77" t="s">
         <v>542</v>
-      </c>
-      <c r="B311" s="77" t="s">
-        <v>543</v>
       </c>
       <c r="C311" s="15" t="s">
         <v>41</v>
@@ -10338,10 +10338,10 @@
     </row>
     <row r="312" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B312" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C312" s="3" t="s">
         <v>9</v>
@@ -10361,7 +10361,7 @@
     </row>
     <row r="313" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B313" s="14" t="s">
         <v>83</v>
@@ -10384,13 +10384,13 @@
     </row>
     <row r="314" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
+        <v>545</v>
+      </c>
+      <c r="B314" s="77" t="s">
         <v>546</v>
       </c>
-      <c r="B314" s="77" t="s">
-        <v>547</v>
-      </c>
       <c r="C314" s="37" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D314" s="37">
         <v>3</v>
@@ -10407,10 +10407,10 @@
     </row>
     <row r="315" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B315" s="77" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C315" s="15" t="s">
         <v>41</v>
@@ -10430,10 +10430,10 @@
     </row>
     <row r="316" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B316" s="14" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C316" s="15" t="s">
         <v>41</v>
@@ -10453,10 +10453,10 @@
     </row>
     <row r="317" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
+        <v>549</v>
+      </c>
+      <c r="B317" s="20" t="s">
         <v>550</v>
-      </c>
-      <c r="B317" s="20" t="s">
-        <v>551</v>
       </c>
       <c r="C317" s="21" t="s">
         <v>58</v>
@@ -10476,10 +10476,10 @@
     </row>
     <row r="318" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
+        <v>551</v>
+      </c>
+      <c r="B318" s="77" t="s">
         <v>552</v>
-      </c>
-      <c r="B318" s="77" t="s">
-        <v>553</v>
       </c>
       <c r="C318" s="15" t="s">
         <v>41</v>
@@ -10499,10 +10499,10 @@
     </row>
     <row r="319" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
+        <v>553</v>
+      </c>
+      <c r="B319" s="8" t="s">
         <v>554</v>
-      </c>
-      <c r="B319" s="8" t="s">
-        <v>555</v>
       </c>
       <c r="C319" s="9" t="s">
         <v>26</v>
@@ -10522,10 +10522,10 @@
     </row>
     <row r="320" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
+        <v>555</v>
+      </c>
+      <c r="B320" s="77" t="s">
         <v>556</v>
-      </c>
-      <c r="B320" s="77" t="s">
-        <v>557</v>
       </c>
       <c r="C320" s="21" t="s">
         <v>58</v>
@@ -10545,10 +10545,10 @@
     </row>
     <row r="321" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B321" s="14" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C321" s="15" t="s">
         <v>41</v>
@@ -10568,10 +10568,10 @@
     </row>
     <row r="322" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
+        <v>558</v>
+      </c>
+      <c r="B322" s="28" t="s">
         <v>559</v>
-      </c>
-      <c r="B322" s="28" t="s">
-        <v>560</v>
       </c>
       <c r="C322" s="29" t="s">
         <v>104</v>
@@ -10591,10 +10591,10 @@
     </row>
     <row r="323" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B323" s="77" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C323" s="29" t="s">
         <v>104</v>
@@ -10614,10 +10614,10 @@
     </row>
     <row r="324" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
+        <v>561</v>
+      </c>
+      <c r="B324" s="77" t="s">
         <v>562</v>
-      </c>
-      <c r="B324" s="77" t="s">
-        <v>563</v>
       </c>
       <c r="C324" s="29" t="s">
         <v>104</v>
@@ -10637,10 +10637,10 @@
     </row>
     <row r="325" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B325" s="77" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C325" s="29" t="s">
         <v>104</v>
@@ -10660,10 +10660,10 @@
     </row>
     <row r="326" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B326" s="77" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C326" s="29" t="s">
         <v>104</v>
@@ -10683,10 +10683,10 @@
     </row>
     <row r="327" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
+        <v>565</v>
+      </c>
+      <c r="B327" s="77" t="s">
         <v>566</v>
-      </c>
-      <c r="B327" s="77" t="s">
-        <v>567</v>
       </c>
       <c r="C327" s="15" t="s">
         <v>41</v>
@@ -10706,10 +10706,10 @@
     </row>
     <row r="328" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
+        <v>567</v>
+      </c>
+      <c r="B328" s="77" t="s">
         <v>568</v>
-      </c>
-      <c r="B328" s="77" t="s">
-        <v>569</v>
       </c>
       <c r="C328" s="21" t="s">
         <v>58</v>
@@ -10729,10 +10729,10 @@
     </row>
     <row r="329" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
+        <v>569</v>
+      </c>
+      <c r="B329" s="77" t="s">
         <v>570</v>
-      </c>
-      <c r="B329" s="77" t="s">
-        <v>571</v>
       </c>
       <c r="C329" s="5" t="s">
         <v>13</v>
@@ -10752,10 +10752,10 @@
     </row>
     <row r="330" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
+        <v>571</v>
+      </c>
+      <c r="B330" s="14" t="s">
         <v>572</v>
-      </c>
-      <c r="B330" s="14" t="s">
-        <v>573</v>
       </c>
       <c r="C330" s="15" t="s">
         <v>41</v>
@@ -10775,10 +10775,10 @@
     </row>
     <row r="331" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
+        <v>573</v>
+      </c>
+      <c r="B331" s="14" t="s">
         <v>574</v>
-      </c>
-      <c r="B331" s="14" t="s">
-        <v>575</v>
       </c>
       <c r="C331" s="15" t="s">
         <v>41</v>
@@ -10798,10 +10798,10 @@
     </row>
     <row r="332" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
+        <v>575</v>
+      </c>
+      <c r="B332" s="8" t="s">
         <v>576</v>
-      </c>
-      <c r="B332" s="8" t="s">
-        <v>577</v>
       </c>
       <c r="C332" s="9" t="s">
         <v>26</v>
@@ -10821,10 +10821,10 @@
     </row>
     <row r="333" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
+        <v>577</v>
+      </c>
+      <c r="B333" s="77" t="s">
         <v>578</v>
-      </c>
-      <c r="B333" s="77" t="s">
-        <v>579</v>
       </c>
       <c r="C333" s="13" t="s">
         <v>36</v>
@@ -10844,13 +10844,13 @@
     </row>
     <row r="334" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
+        <v>579</v>
+      </c>
+      <c r="B334" s="36" t="s">
         <v>580</v>
       </c>
-      <c r="B334" s="36" t="s">
-        <v>581</v>
-      </c>
       <c r="C334" s="37" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D334" s="37">
         <v>20</v>
@@ -10867,10 +10867,10 @@
     </row>
     <row r="335" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
+        <v>581</v>
+      </c>
+      <c r="B335" s="34" t="s">
         <v>582</v>
-      </c>
-      <c r="B335" s="34" t="s">
-        <v>583</v>
       </c>
       <c r="C335" s="35" t="s">
         <v>159</v>
@@ -10890,10 +10890,10 @@
     </row>
     <row r="336" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
+        <v>583</v>
+      </c>
+      <c r="B336" s="14" t="s">
         <v>584</v>
-      </c>
-      <c r="B336" s="14" t="s">
-        <v>585</v>
       </c>
       <c r="C336" s="15" t="s">
         <v>41</v>
@@ -10913,7 +10913,7 @@
     </row>
     <row r="337" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B337" s="14" t="s">
         <v>83</v>
@@ -10936,7 +10936,7 @@
     </row>
     <row r="338" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B338" s="2" t="s">
         <v>83</v>
@@ -10959,10 +10959,10 @@
     </row>
     <row r="339" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
+        <v>587</v>
+      </c>
+      <c r="B339" s="12" t="s">
         <v>588</v>
-      </c>
-      <c r="B339" s="12" t="s">
-        <v>589</v>
       </c>
       <c r="C339" s="13" t="s">
         <v>36</v>
@@ -10982,7 +10982,7 @@
     </row>
     <row r="340" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B340" s="28" t="s">
         <v>156</v>
@@ -11005,7 +11005,7 @@
     </row>
     <row r="341" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B341" s="26" t="s">
         <v>83</v>
@@ -11028,7 +11028,7 @@
     </row>
     <row r="342" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B342" s="77" t="s">
         <v>148</v>
@@ -11051,10 +11051,10 @@
     </row>
     <row r="343" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
+        <v>592</v>
+      </c>
+      <c r="B343" s="26" t="s">
         <v>593</v>
-      </c>
-      <c r="B343" s="26" t="s">
-        <v>594</v>
       </c>
       <c r="C343" s="27" t="s">
         <v>92</v>
@@ -11074,10 +11074,10 @@
     </row>
     <row r="344" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
+        <v>594</v>
+      </c>
+      <c r="B344" s="77" t="s">
         <v>595</v>
-      </c>
-      <c r="B344" s="77" t="s">
-        <v>596</v>
       </c>
       <c r="C344" s="27" t="s">
         <v>92</v>
@@ -11097,7 +11097,7 @@
     </row>
     <row r="345" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B345" s="26" t="s">
         <v>83</v>
@@ -11120,10 +11120,10 @@
     </row>
     <row r="346" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
+        <v>597</v>
+      </c>
+      <c r="B346" s="14" t="s">
         <v>598</v>
-      </c>
-      <c r="B346" s="14" t="s">
-        <v>599</v>
       </c>
       <c r="C346" s="15" t="s">
         <v>41</v>
@@ -11143,10 +11143,10 @@
     </row>
     <row r="347" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
+        <v>599</v>
+      </c>
+      <c r="B347" s="26" t="s">
         <v>600</v>
-      </c>
-      <c r="B347" s="26" t="s">
-        <v>601</v>
       </c>
       <c r="C347" s="27" t="s">
         <v>92</v>
@@ -11166,10 +11166,10 @@
     </row>
     <row r="348" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
+        <v>601</v>
+      </c>
+      <c r="B348" s="14" t="s">
         <v>602</v>
-      </c>
-      <c r="B348" s="14" t="s">
-        <v>603</v>
       </c>
       <c r="C348" s="15" t="s">
         <v>41</v>
@@ -11189,10 +11189,10 @@
     </row>
     <row r="349" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
+        <v>603</v>
+      </c>
+      <c r="B349" s="22" t="s">
         <v>604</v>
-      </c>
-      <c r="B349" s="22" t="s">
-        <v>605</v>
       </c>
       <c r="C349" s="23" t="s">
         <v>70</v>
@@ -11212,7 +11212,7 @@
     </row>
     <row r="350" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B350" s="6" t="s">
         <v>83</v>
@@ -11235,10 +11235,10 @@
     </row>
     <row r="351" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
+        <v>606</v>
+      </c>
+      <c r="B351" s="14" t="s">
         <v>607</v>
-      </c>
-      <c r="B351" s="14" t="s">
-        <v>608</v>
       </c>
       <c r="C351" s="15" t="s">
         <v>41</v>
@@ -11258,10 +11258,10 @@
     </row>
     <row r="352" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B352" s="77" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C352" s="27" t="s">
         <v>92</v>
@@ -11281,7 +11281,7 @@
     </row>
     <row r="353" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B353" s="14" t="s">
         <v>65</v>
@@ -11304,10 +11304,10 @@
     </row>
     <row r="354" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
+        <v>610</v>
+      </c>
+      <c r="B354" s="77" t="s">
         <v>611</v>
-      </c>
-      <c r="B354" s="77" t="s">
-        <v>612</v>
       </c>
       <c r="C354" s="15" t="s">
         <v>41</v>
@@ -11327,10 +11327,10 @@
     </row>
     <row r="355" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B355" s="77" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C355" s="75" t="s">
         <v>104</v>

</xml_diff>

<commit_message>
Added 2 variable moves. Added ability data.
</commit_message>
<xml_diff>
--- a/data/gen3moves.xlsx
+++ b/data/gen3moves.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Projects\EKhelper\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BCAF9A-D6C5-4924-A8B8-D033493CC325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078FEFC6-4562-4CFD-B488-C549843F4DC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -320,9 +320,6 @@
     <t>Bullet Seed</t>
   </si>
   <si>
-    <t>Always hits twice.</t>
-  </si>
-  <si>
     <t>Calm Mind</t>
   </si>
   <si>
@@ -1878,6 +1875,9 @@
   </si>
   <si>
     <t>Priority +1 move</t>
+  </si>
+  <si>
+    <t>Always hits twice. (2x25)</t>
   </si>
 </sst>
 </file>
@@ -3184,8 +3184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G355"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3431,7 +3431,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="77" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>35</v>
@@ -3500,7 +3500,7 @@
         <v>42</v>
       </c>
       <c r="B14" s="77" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>43</v>
@@ -4052,16 +4052,16 @@
         <v>94</v>
       </c>
       <c r="B38" s="77" t="s">
-        <v>95</v>
+        <v>614</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D38" s="3">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E38" s="3">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="F38" s="39">
         <v>1</v>
@@ -4072,10 +4072,10 @@
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39" s="77" t="s">
         <v>96</v>
-      </c>
-      <c r="B39" s="77" t="s">
-        <v>97</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>26</v>
@@ -4095,10 +4095,10 @@
     </row>
     <row r="40" spans="1:7" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" s="14" t="s">
         <v>98</v>
-      </c>
-      <c r="B40" s="14" t="s">
-        <v>99</v>
       </c>
       <c r="C40" s="15" t="s">
         <v>40</v>
@@ -4118,13 +4118,13 @@
     </row>
     <row r="41" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>99</v>
+      </c>
+      <c r="B41" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="B41" s="28" t="s">
+      <c r="C41" s="29" t="s">
         <v>101</v>
-      </c>
-      <c r="C41" s="29" t="s">
-        <v>102</v>
       </c>
       <c r="D41" s="29">
         <v>20</v>
@@ -4141,10 +4141,10 @@
     </row>
     <row r="42" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>102</v>
+      </c>
+      <c r="B42" s="77" t="s">
         <v>103</v>
-      </c>
-      <c r="B42" s="77" t="s">
-        <v>104</v>
       </c>
       <c r="C42" s="15" t="s">
         <v>40</v>
@@ -4164,7 +4164,7 @@
     </row>
     <row r="43" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B43" s="26" t="s">
         <v>63</v>
@@ -4187,7 +4187,7 @@
     </row>
     <row r="44" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B44" s="77" t="s">
         <v>50</v>
@@ -4210,10 +4210,10 @@
     </row>
     <row r="45" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>106</v>
+      </c>
+      <c r="B45" s="77" t="s">
         <v>107</v>
-      </c>
-      <c r="B45" s="77" t="s">
-        <v>108</v>
       </c>
       <c r="C45" s="17" t="s">
         <v>43</v>
@@ -4233,10 +4233,10 @@
     </row>
     <row r="46" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>108</v>
+      </c>
+      <c r="B46" s="77" t="s">
         <v>109</v>
-      </c>
-      <c r="B46" s="77" t="s">
-        <v>110</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>26</v>
@@ -4256,7 +4256,7 @@
     </row>
     <row r="47" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B47" s="77" t="s">
         <v>89</v>
@@ -4279,10 +4279,10 @@
     </row>
     <row r="48" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>111</v>
+      </c>
+      <c r="B48" s="14" t="s">
         <v>112</v>
-      </c>
-      <c r="B48" s="14" t="s">
-        <v>113</v>
       </c>
       <c r="C48" s="15" t="s">
         <v>40</v>
@@ -4302,10 +4302,10 @@
     </row>
     <row r="49" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>113</v>
+      </c>
+      <c r="B49" s="14" t="s">
         <v>114</v>
-      </c>
-      <c r="B49" s="14" t="s">
-        <v>115</v>
       </c>
       <c r="C49" s="15" t="s">
         <v>40</v>
@@ -4325,10 +4325,10 @@
     </row>
     <row r="50" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>115</v>
+      </c>
+      <c r="B50" s="77" t="s">
         <v>116</v>
-      </c>
-      <c r="B50" s="77" t="s">
-        <v>117</v>
       </c>
       <c r="C50" s="9" t="s">
         <v>26</v>
@@ -4348,10 +4348,10 @@
     </row>
     <row r="51" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>117</v>
+      </c>
+      <c r="B51" s="77" t="s">
         <v>118</v>
-      </c>
-      <c r="B51" s="77" t="s">
-        <v>119</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>9</v>
@@ -4371,10 +4371,10 @@
     </row>
     <row r="52" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>119</v>
+      </c>
+      <c r="B52" s="77" t="s">
         <v>120</v>
-      </c>
-      <c r="B52" s="77" t="s">
-        <v>121</v>
       </c>
       <c r="C52" s="13" t="s">
         <v>35</v>
@@ -4394,10 +4394,10 @@
     </row>
     <row r="53" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>121</v>
+      </c>
+      <c r="B53" s="14" t="s">
         <v>122</v>
-      </c>
-      <c r="B53" s="14" t="s">
-        <v>123</v>
       </c>
       <c r="C53" s="15" t="s">
         <v>40</v>
@@ -4417,7 +4417,7 @@
     </row>
     <row r="54" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B54" s="77" t="s">
         <v>23</v>
@@ -4440,7 +4440,7 @@
     </row>
     <row r="55" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B55" s="77" t="s">
         <v>23</v>
@@ -4463,10 +4463,10 @@
     </row>
     <row r="56" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>125</v>
+      </c>
+      <c r="B56" s="77" t="s">
         <v>126</v>
-      </c>
-      <c r="B56" s="77" t="s">
-        <v>127</v>
       </c>
       <c r="C56" s="21" t="s">
         <v>56</v>
@@ -4486,10 +4486,10 @@
     </row>
     <row r="57" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>127</v>
+      </c>
+      <c r="B57" s="77" t="s">
         <v>128</v>
-      </c>
-      <c r="B57" s="77" t="s">
-        <v>129</v>
       </c>
       <c r="C57" s="15" t="s">
         <v>40</v>
@@ -4509,10 +4509,10 @@
     </row>
     <row r="58" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
+        <v>129</v>
+      </c>
+      <c r="B58" s="30" t="s">
         <v>130</v>
-      </c>
-      <c r="B58" s="30" t="s">
-        <v>131</v>
       </c>
       <c r="C58" s="31" t="s">
         <v>40</v>
@@ -4532,7 +4532,7 @@
     </row>
     <row r="59" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B59" s="14" t="s">
         <v>81</v>
@@ -4555,10 +4555,10 @@
     </row>
     <row r="60" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
+        <v>132</v>
+      </c>
+      <c r="B60" s="14" t="s">
         <v>133</v>
-      </c>
-      <c r="B60" s="14" t="s">
-        <v>134</v>
       </c>
       <c r="C60" s="15" t="s">
         <v>40</v>
@@ -4578,10 +4578,10 @@
     </row>
     <row r="61" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
+        <v>134</v>
+      </c>
+      <c r="B61" s="77" t="s">
         <v>135</v>
-      </c>
-      <c r="B61" s="77" t="s">
-        <v>136</v>
       </c>
       <c r="C61" s="17" t="s">
         <v>43</v>
@@ -4601,10 +4601,10 @@
     </row>
     <row r="62" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
+        <v>136</v>
+      </c>
+      <c r="B62" s="12" t="s">
         <v>137</v>
-      </c>
-      <c r="B62" s="12" t="s">
-        <v>138</v>
       </c>
       <c r="C62" s="13" t="s">
         <v>35</v>
@@ -4624,10 +4624,10 @@
     </row>
     <row r="63" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
+        <v>138</v>
+      </c>
+      <c r="B63" s="24" t="s">
         <v>139</v>
-      </c>
-      <c r="B63" s="24" t="s">
-        <v>140</v>
       </c>
       <c r="C63" s="25" t="s">
         <v>79</v>
@@ -4647,10 +4647,10 @@
     </row>
     <row r="64" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
+        <v>140</v>
+      </c>
+      <c r="B64" s="77" t="s">
         <v>141</v>
-      </c>
-      <c r="B64" s="77" t="s">
-        <v>142</v>
       </c>
       <c r="C64" s="15" t="s">
         <v>40</v>
@@ -4670,10 +4670,10 @@
     </row>
     <row r="65" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
+        <v>142</v>
+      </c>
+      <c r="B65" s="26" t="s">
         <v>143</v>
-      </c>
-      <c r="B65" s="26" t="s">
-        <v>144</v>
       </c>
       <c r="C65" s="27" t="s">
         <v>90</v>
@@ -4693,10 +4693,10 @@
     </row>
     <row r="66" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
+        <v>144</v>
+      </c>
+      <c r="B66" s="77" t="s">
         <v>145</v>
-      </c>
-      <c r="B66" s="77" t="s">
-        <v>146</v>
       </c>
       <c r="C66" s="15" t="s">
         <v>40</v>
@@ -4716,13 +4716,13 @@
     </row>
     <row r="67" spans="1:7" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
+        <v>146</v>
+      </c>
+      <c r="B67" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="B67" s="32" t="s">
+      <c r="C67" s="33" t="s">
         <v>148</v>
-      </c>
-      <c r="C67" s="33" t="s">
-        <v>149</v>
       </c>
       <c r="D67" s="33">
         <v>5</v>
@@ -4739,7 +4739,7 @@
     </row>
     <row r="68" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B68" s="77" t="s">
         <v>83</v>
@@ -4762,10 +4762,10 @@
     </row>
     <row r="69" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
+        <v>150</v>
+      </c>
+      <c r="B69" s="77" t="s">
         <v>151</v>
-      </c>
-      <c r="B69" s="77" t="s">
-        <v>152</v>
       </c>
       <c r="C69" s="15" t="s">
         <v>40</v>
@@ -4785,10 +4785,10 @@
     </row>
     <row r="70" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
+        <v>152</v>
+      </c>
+      <c r="B70" s="14" t="s">
         <v>153</v>
-      </c>
-      <c r="B70" s="14" t="s">
-        <v>154</v>
       </c>
       <c r="C70" s="15" t="s">
         <v>40</v>
@@ -4808,7 +4808,7 @@
     </row>
     <row r="71" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B71" s="77" t="s">
         <v>50</v>
@@ -4831,13 +4831,13 @@
     </row>
     <row r="72" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B72" s="34" t="s">
         <v>81</v>
       </c>
       <c r="C72" s="35" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D72" s="35">
         <v>24</v>
@@ -4854,13 +4854,13 @@
     </row>
     <row r="73" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
+        <v>157</v>
+      </c>
+      <c r="B73" s="77" t="s">
         <v>158</v>
       </c>
-      <c r="B73" s="77" t="s">
-        <v>159</v>
-      </c>
       <c r="C73" s="35" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D73" s="35">
         <v>3</v>
@@ -4877,19 +4877,19 @@
     </row>
     <row r="74" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
+        <v>159</v>
+      </c>
+      <c r="B74" s="34" t="s">
         <v>160</v>
       </c>
-      <c r="B74" s="34" t="s">
+      <c r="C74" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="D74" s="35">
+        <v>10</v>
+      </c>
+      <c r="E74" s="35" t="s">
         <v>161</v>
-      </c>
-      <c r="C74" s="35" t="s">
-        <v>157</v>
-      </c>
-      <c r="D74" s="35">
-        <v>10</v>
-      </c>
-      <c r="E74" s="35" t="s">
-        <v>162</v>
       </c>
       <c r="F74" s="61">
         <v>1</v>
@@ -4900,13 +4900,13 @@
     </row>
     <row r="75" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B75" s="77" t="s">
         <v>76</v>
       </c>
       <c r="C75" s="35" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D75" s="35">
         <v>20</v>
@@ -4923,10 +4923,10 @@
     </row>
     <row r="76" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
+        <v>163</v>
+      </c>
+      <c r="B76" s="77" t="s">
         <v>164</v>
-      </c>
-      <c r="B76" s="77" t="s">
-        <v>165</v>
       </c>
       <c r="C76" s="9" t="s">
         <v>26</v>
@@ -4946,7 +4946,7 @@
     </row>
     <row r="77" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B77" s="6" t="s">
         <v>81</v>
@@ -4969,10 +4969,10 @@
     </row>
     <row r="78" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B78" s="77" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C78" s="13" t="s">
         <v>35</v>
@@ -4992,10 +4992,10 @@
     </row>
     <row r="79" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
+        <v>167</v>
+      </c>
+      <c r="B79" s="77" t="s">
         <v>168</v>
-      </c>
-      <c r="B79" s="77" t="s">
-        <v>169</v>
       </c>
       <c r="C79" s="25" t="s">
         <v>79</v>
@@ -5015,10 +5015,10 @@
     </row>
     <row r="80" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
+        <v>169</v>
+      </c>
+      <c r="B80" s="77" t="s">
         <v>170</v>
-      </c>
-      <c r="B80" s="77" t="s">
-        <v>171</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>9</v>
@@ -5038,10 +5038,10 @@
     </row>
     <row r="81" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
+        <v>171</v>
+      </c>
+      <c r="B81" s="77" t="s">
         <v>172</v>
-      </c>
-      <c r="B81" s="77" t="s">
-        <v>173</v>
       </c>
       <c r="C81" s="23" t="s">
         <v>68</v>
@@ -5061,10 +5061,10 @@
     </row>
     <row r="82" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
+        <v>173</v>
+      </c>
+      <c r="B82" s="77" t="s">
         <v>174</v>
-      </c>
-      <c r="B82" s="77" t="s">
-        <v>175</v>
       </c>
       <c r="C82" s="15" t="s">
         <v>40</v>
@@ -5084,10 +5084,10 @@
     </row>
     <row r="83" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
+        <v>175</v>
+      </c>
+      <c r="B83" s="14" t="s">
         <v>176</v>
-      </c>
-      <c r="B83" s="14" t="s">
-        <v>177</v>
       </c>
       <c r="C83" s="15" t="s">
         <v>40</v>
@@ -5107,10 +5107,10 @@
     </row>
     <row r="84" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
+        <v>177</v>
+      </c>
+      <c r="B84" s="14" t="s">
         <v>178</v>
-      </c>
-      <c r="B84" s="14" t="s">
-        <v>179</v>
       </c>
       <c r="C84" s="15" t="s">
         <v>40</v>
@@ -5130,10 +5130,10 @@
     </row>
     <row r="85" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
+        <v>179</v>
+      </c>
+      <c r="B85" s="77" t="s">
         <v>180</v>
-      </c>
-      <c r="B85" s="77" t="s">
-        <v>181</v>
       </c>
       <c r="C85" s="23" t="s">
         <v>68</v>
@@ -5153,10 +5153,10 @@
     </row>
     <row r="86" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
+        <v>181</v>
+      </c>
+      <c r="B86" s="77" t="s">
         <v>182</v>
-      </c>
-      <c r="B86" s="77" t="s">
-        <v>183</v>
       </c>
       <c r="C86" s="15" t="s">
         <v>40</v>
@@ -5176,7 +5176,7 @@
     </row>
     <row r="87" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B87" s="77" t="s">
         <v>78</v>
@@ -5199,10 +5199,10 @@
     </row>
     <row r="88" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
+        <v>184</v>
+      </c>
+      <c r="B88" s="77" t="s">
         <v>185</v>
-      </c>
-      <c r="B88" s="77" t="s">
-        <v>186</v>
       </c>
       <c r="C88" s="15" t="s">
         <v>40</v>
@@ -5222,10 +5222,10 @@
     </row>
     <row r="89" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
+        <v>186</v>
+      </c>
+      <c r="B89" s="14" t="s">
         <v>187</v>
-      </c>
-      <c r="B89" s="14" t="s">
-        <v>188</v>
       </c>
       <c r="C89" s="15" t="s">
         <v>40</v>
@@ -5245,7 +5245,7 @@
     </row>
     <row r="90" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B90" s="20" t="s">
         <v>19</v>
@@ -5268,10 +5268,10 @@
     </row>
     <row r="91" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
+        <v>189</v>
+      </c>
+      <c r="B91" s="77" t="s">
         <v>190</v>
-      </c>
-      <c r="B91" s="77" t="s">
-        <v>191</v>
       </c>
       <c r="C91" s="15" t="s">
         <v>40</v>
@@ -5291,10 +5291,10 @@
     </row>
     <row r="92" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
+        <v>191</v>
+      </c>
+      <c r="B92" s="77" t="s">
         <v>192</v>
-      </c>
-      <c r="B92" s="77" t="s">
-        <v>193</v>
       </c>
       <c r="C92" s="21" t="s">
         <v>56</v>
@@ -5314,10 +5314,10 @@
     </row>
     <row r="93" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
+        <v>193</v>
+      </c>
+      <c r="B93" s="14" t="s">
         <v>194</v>
-      </c>
-      <c r="B93" s="14" t="s">
-        <v>195</v>
       </c>
       <c r="C93" s="15" t="s">
         <v>40</v>
@@ -5337,10 +5337,10 @@
     </row>
     <row r="94" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B94" s="77" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C94" s="7" t="s">
         <v>20</v>
@@ -5360,10 +5360,10 @@
     </row>
     <row r="95" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B95" s="77" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C95" s="23" t="s">
         <v>68</v>
@@ -5383,10 +5383,10 @@
     </row>
     <row r="96" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B96" s="77" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C96" s="23" t="s">
         <v>68</v>
@@ -5406,7 +5406,7 @@
     </row>
     <row r="97" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B97" s="22" t="s">
         <v>63</v>
@@ -5429,10 +5429,10 @@
     </row>
     <row r="98" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
+        <v>199</v>
+      </c>
+      <c r="B98" s="77" t="s">
         <v>200</v>
-      </c>
-      <c r="B98" s="77" t="s">
-        <v>201</v>
       </c>
       <c r="C98" s="25" t="s">
         <v>79</v>
@@ -5452,10 +5452,10 @@
     </row>
     <row r="99" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
+        <v>201</v>
+      </c>
+      <c r="B99" s="77" t="s">
         <v>202</v>
-      </c>
-      <c r="B99" s="77" t="s">
-        <v>203</v>
       </c>
       <c r="C99" s="15" t="s">
         <v>40</v>
@@ -5464,7 +5464,7 @@
         <v>5</v>
       </c>
       <c r="E99" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F99" s="49">
         <v>1</v>
@@ -5475,10 +5475,10 @@
     </row>
     <row r="100" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
+        <v>204</v>
+      </c>
+      <c r="B100" s="22" t="s">
         <v>205</v>
-      </c>
-      <c r="B100" s="22" t="s">
-        <v>206</v>
       </c>
       <c r="C100" s="23" t="s">
         <v>68</v>
@@ -5498,10 +5498,10 @@
     </row>
     <row r="101" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B101" s="77" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C101" s="23" t="s">
         <v>68</v>
@@ -5521,10 +5521,10 @@
     </row>
     <row r="102" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
+        <v>207</v>
+      </c>
+      <c r="B102" s="77" t="s">
         <v>208</v>
-      </c>
-      <c r="B102" s="77" t="s">
-        <v>209</v>
       </c>
       <c r="C102" s="15" t="s">
         <v>40</v>
@@ -5544,10 +5544,10 @@
     </row>
     <row r="103" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
+        <v>209</v>
+      </c>
+      <c r="B103" s="20" t="s">
         <v>210</v>
-      </c>
-      <c r="B103" s="20" t="s">
-        <v>211</v>
       </c>
       <c r="C103" s="21" t="s">
         <v>56</v>
@@ -5567,10 +5567,10 @@
     </row>
     <row r="104" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
+        <v>211</v>
+      </c>
+      <c r="B104" s="6" t="s">
         <v>212</v>
-      </c>
-      <c r="B104" s="6" t="s">
-        <v>213</v>
       </c>
       <c r="C104" s="7" t="s">
         <v>20</v>
@@ -5590,10 +5590,10 @@
     </row>
     <row r="105" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
+        <v>213</v>
+      </c>
+      <c r="B105" s="77" t="s">
         <v>214</v>
-      </c>
-      <c r="B105" s="77" t="s">
-        <v>215</v>
       </c>
       <c r="C105" s="15" t="s">
         <v>40</v>
@@ -5613,10 +5613,10 @@
     </row>
     <row r="106" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
+        <v>215</v>
+      </c>
+      <c r="B106" s="77" t="s">
         <v>216</v>
-      </c>
-      <c r="B106" s="77" t="s">
-        <v>217</v>
       </c>
       <c r="C106" s="13" t="s">
         <v>35</v>
@@ -5636,10 +5636,10 @@
     </row>
     <row r="107" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
+        <v>217</v>
+      </c>
+      <c r="B107" s="77" t="s">
         <v>218</v>
-      </c>
-      <c r="B107" s="77" t="s">
-        <v>219</v>
       </c>
       <c r="C107" s="15" t="s">
         <v>40</v>
@@ -5659,10 +5659,10 @@
     </row>
     <row r="108" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
+        <v>219</v>
+      </c>
+      <c r="B108" s="14" t="s">
         <v>220</v>
-      </c>
-      <c r="B108" s="14" t="s">
-        <v>221</v>
       </c>
       <c r="C108" s="15" t="s">
         <v>40</v>
@@ -5682,7 +5682,7 @@
     </row>
     <row r="109" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B109" s="77" t="s">
         <v>67</v>
@@ -5705,10 +5705,10 @@
     </row>
     <row r="110" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
+        <v>222</v>
+      </c>
+      <c r="B110" s="77" t="s">
         <v>223</v>
-      </c>
-      <c r="B110" s="77" t="s">
-        <v>224</v>
       </c>
       <c r="C110" s="15" t="s">
         <v>40</v>
@@ -5728,7 +5728,7 @@
     </row>
     <row r="111" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B111" s="77" t="s">
         <v>50</v>
@@ -5751,13 +5751,13 @@
     </row>
     <row r="112" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
+        <v>225</v>
+      </c>
+      <c r="B112" s="36" t="s">
+        <v>610</v>
+      </c>
+      <c r="C112" s="37" t="s">
         <v>226</v>
-      </c>
-      <c r="B112" s="36" t="s">
-        <v>611</v>
-      </c>
-      <c r="C112" s="37" t="s">
-        <v>227</v>
       </c>
       <c r="D112" s="37">
         <v>15</v>
@@ -5774,7 +5774,7 @@
     </row>
     <row r="113" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B113" s="77" t="s">
         <v>50</v>
@@ -5797,10 +5797,10 @@
     </row>
     <row r="114" spans="1:7" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
+        <v>228</v>
+      </c>
+      <c r="B114" s="8" t="s">
         <v>229</v>
-      </c>
-      <c r="B114" s="8" t="s">
-        <v>230</v>
       </c>
       <c r="C114" s="9" t="s">
         <v>26</v>
@@ -5820,7 +5820,7 @@
     </row>
     <row r="115" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>8</v>
@@ -5843,10 +5843,10 @@
     </row>
     <row r="116" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
+        <v>231</v>
+      </c>
+      <c r="B116" s="77" t="s">
         <v>232</v>
-      </c>
-      <c r="B116" s="77" t="s">
-        <v>233</v>
       </c>
       <c r="C116" s="15" t="s">
         <v>40</v>
@@ -5866,10 +5866,10 @@
     </row>
     <row r="117" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
+        <v>233</v>
+      </c>
+      <c r="B117" s="77" t="s">
         <v>234</v>
-      </c>
-      <c r="B117" s="77" t="s">
-        <v>235</v>
       </c>
       <c r="C117" s="3" t="s">
         <v>9</v>
@@ -5889,10 +5889,10 @@
     </row>
     <row r="118" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
+        <v>235</v>
+      </c>
+      <c r="B118" s="77" t="s">
         <v>236</v>
-      </c>
-      <c r="B118" s="77" t="s">
-        <v>237</v>
       </c>
       <c r="C118" s="15" t="s">
         <v>40</v>
@@ -5912,10 +5912,10 @@
     </row>
     <row r="119" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
+        <v>237</v>
+      </c>
+      <c r="B119" s="77" t="s">
         <v>238</v>
-      </c>
-      <c r="B119" s="77" t="s">
-        <v>239</v>
       </c>
       <c r="C119" s="15" t="s">
         <v>40</v>
@@ -5935,10 +5935,10 @@
     </row>
     <row r="120" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
+        <v>239</v>
+      </c>
+      <c r="B120" s="16" t="s">
         <v>240</v>
-      </c>
-      <c r="B120" s="16" t="s">
-        <v>241</v>
       </c>
       <c r="C120" s="17" t="s">
         <v>43</v>
@@ -5958,10 +5958,10 @@
     </row>
     <row r="121" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
+        <v>241</v>
+      </c>
+      <c r="B121" s="77" t="s">
         <v>242</v>
-      </c>
-      <c r="B121" s="77" t="s">
-        <v>243</v>
       </c>
       <c r="C121" s="15" t="s">
         <v>40</v>
@@ -5970,7 +5970,7 @@
         <v>5</v>
       </c>
       <c r="E121" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F121" s="49">
         <v>0.3</v>
@@ -5981,10 +5981,10 @@
     </row>
     <row r="122" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
+        <v>244</v>
+      </c>
+      <c r="B122" s="6" t="s">
         <v>245</v>
-      </c>
-      <c r="B122" s="6" t="s">
-        <v>246</v>
       </c>
       <c r="C122" s="7" t="s">
         <v>20</v>
@@ -6004,10 +6004,10 @@
     </row>
     <row r="123" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
+        <v>246</v>
+      </c>
+      <c r="B123" s="18" t="s">
         <v>247</v>
-      </c>
-      <c r="B123" s="18" t="s">
-        <v>248</v>
       </c>
       <c r="C123" s="19" t="s">
         <v>48</v>
@@ -6027,10 +6027,10 @@
     </row>
     <row r="124" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
+        <v>248</v>
+      </c>
+      <c r="B124" s="77" t="s">
         <v>249</v>
-      </c>
-      <c r="B124" s="77" t="s">
-        <v>250</v>
       </c>
       <c r="C124" s="15" t="s">
         <v>40</v>
@@ -6050,10 +6050,10 @@
     </row>
     <row r="125" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
+        <v>250</v>
+      </c>
+      <c r="B125" s="77" t="s">
         <v>251</v>
-      </c>
-      <c r="B125" s="77" t="s">
-        <v>252</v>
       </c>
       <c r="C125" s="19" t="s">
         <v>48</v>
@@ -6073,7 +6073,7 @@
     </row>
     <row r="126" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B126" s="77" t="s">
         <v>65</v>
@@ -6096,10 +6096,10 @@
     </row>
     <row r="127" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
+        <v>253</v>
+      </c>
+      <c r="B127" s="14" t="s">
         <v>254</v>
-      </c>
-      <c r="B127" s="14" t="s">
-        <v>255</v>
       </c>
       <c r="C127" s="15" t="s">
         <v>40</v>
@@ -6119,10 +6119,10 @@
     </row>
     <row r="128" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B128" s="77" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C128" s="23" t="s">
         <v>68</v>
@@ -6142,10 +6142,10 @@
     </row>
     <row r="129" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
+        <v>256</v>
+      </c>
+      <c r="B129" s="77" t="s">
         <v>257</v>
-      </c>
-      <c r="B129" s="77" t="s">
-        <v>258</v>
       </c>
       <c r="C129" s="15" t="s">
         <v>40</v>
@@ -6165,10 +6165,10 @@
     </row>
     <row r="130" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
+        <v>258</v>
+      </c>
+      <c r="B130" s="12" t="s">
         <v>259</v>
-      </c>
-      <c r="B130" s="12" t="s">
-        <v>260</v>
       </c>
       <c r="C130" s="13" t="s">
         <v>35</v>
@@ -6188,10 +6188,10 @@
     </row>
     <row r="131" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
+        <v>260</v>
+      </c>
+      <c r="B131" s="14" t="s">
         <v>261</v>
-      </c>
-      <c r="B131" s="14" t="s">
-        <v>262</v>
       </c>
       <c r="C131" s="15" t="s">
         <v>40</v>
@@ -6200,7 +6200,7 @@
         <v>15</v>
       </c>
       <c r="E131" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F131" s="49">
         <v>1</v>
@@ -6211,7 +6211,7 @@
     </row>
     <row r="132" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B132" s="14" t="s">
         <v>81</v>
@@ -6234,10 +6234,10 @@
     </row>
     <row r="133" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
+        <v>263</v>
+      </c>
+      <c r="B133" s="77" t="s">
         <v>264</v>
-      </c>
-      <c r="B133" s="77" t="s">
-        <v>265</v>
       </c>
       <c r="C133" s="15" t="s">
         <v>40</v>
@@ -6257,10 +6257,10 @@
     </row>
     <row r="134" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
+        <v>265</v>
+      </c>
+      <c r="B134" s="77" t="s">
         <v>266</v>
-      </c>
-      <c r="B134" s="77" t="s">
-        <v>267</v>
       </c>
       <c r="C134" s="15" t="s">
         <v>40</v>
@@ -6280,7 +6280,7 @@
     </row>
     <row r="135" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B135" s="77" t="s">
         <v>67</v>
@@ -6303,7 +6303,7 @@
     </row>
     <row r="136" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B136" s="26" t="s">
         <v>81</v>
@@ -6326,7 +6326,7 @@
     </row>
     <row r="137" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B137" s="77" t="s">
         <v>67</v>
@@ -6349,7 +6349,7 @@
     </row>
     <row r="138" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B138" s="77" t="s">
         <v>78</v>
@@ -6372,10 +6372,10 @@
     </row>
     <row r="139" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
+        <v>271</v>
+      </c>
+      <c r="B139" s="14" t="s">
         <v>272</v>
-      </c>
-      <c r="B139" s="14" t="s">
-        <v>273</v>
       </c>
       <c r="C139" s="15" t="s">
         <v>40</v>
@@ -6395,10 +6395,10 @@
     </row>
     <row r="140" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B140" s="77" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C140" s="9" t="s">
         <v>26</v>
@@ -6418,10 +6418,10 @@
     </row>
     <row r="141" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
+        <v>274</v>
+      </c>
+      <c r="B141" s="18" t="s">
         <v>275</v>
-      </c>
-      <c r="B141" s="18" t="s">
-        <v>276</v>
       </c>
       <c r="C141" s="19" t="s">
         <v>48</v>
@@ -6441,7 +6441,7 @@
     </row>
     <row r="142" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B142" s="77" t="s">
         <v>72</v>
@@ -6464,7 +6464,7 @@
     </row>
     <row r="143" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B143" s="77" t="s">
         <v>72</v>
@@ -6487,10 +6487,10 @@
     </row>
     <row r="144" spans="1:7" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B144" s="77" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C144" s="19" t="s">
         <v>48</v>
@@ -6510,10 +6510,10 @@
     </row>
     <row r="145" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
+        <v>279</v>
+      </c>
+      <c r="B145" s="77" t="s">
         <v>280</v>
-      </c>
-      <c r="B145" s="77" t="s">
-        <v>281</v>
       </c>
       <c r="C145" s="19" t="s">
         <v>48</v>
@@ -6533,10 +6533,10 @@
     </row>
     <row r="146" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
+        <v>281</v>
+      </c>
+      <c r="B146" s="8" t="s">
         <v>282</v>
-      </c>
-      <c r="B146" s="8" t="s">
-        <v>283</v>
       </c>
       <c r="C146" s="9" t="s">
         <v>26</v>
@@ -6556,10 +6556,10 @@
     </row>
     <row r="147" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
+        <v>283</v>
+      </c>
+      <c r="B147" s="2" t="s">
         <v>284</v>
-      </c>
-      <c r="B147" s="2" t="s">
-        <v>285</v>
       </c>
       <c r="C147" s="3" t="s">
         <v>9</v>
@@ -6579,13 +6579,13 @@
     </row>
     <row r="148" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B148" s="77" t="s">
         <v>15</v>
       </c>
       <c r="C148" s="33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D148" s="33">
         <v>15</v>
@@ -6602,13 +6602,13 @@
     </row>
     <row r="149" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
+        <v>286</v>
+      </c>
+      <c r="B149" s="77" t="s">
         <v>287</v>
       </c>
-      <c r="B149" s="77" t="s">
-        <v>288</v>
-      </c>
       <c r="C149" s="33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D149" s="33">
         <v>24</v>
@@ -6625,10 +6625,10 @@
     </row>
     <row r="150" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B150" s="12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C150" s="13" t="s">
         <v>35</v>
@@ -6648,7 +6648,7 @@
     </row>
     <row r="151" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B151" s="77" t="s">
         <v>23</v>
@@ -6671,10 +6671,10 @@
     </row>
     <row r="152" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B152" s="77" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C152" s="9" t="s">
         <v>26</v>
@@ -6694,10 +6694,10 @@
     </row>
     <row r="153" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
+        <v>291</v>
+      </c>
+      <c r="B153" s="20" t="s">
         <v>292</v>
-      </c>
-      <c r="B153" s="20" t="s">
-        <v>293</v>
       </c>
       <c r="C153" s="21" t="s">
         <v>56</v>
@@ -6717,7 +6717,7 @@
     </row>
     <row r="154" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B154" s="77" t="s">
         <v>23</v>
@@ -6740,13 +6740,13 @@
     </row>
     <row r="155" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B155" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C155" s="37" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D155" s="37">
         <v>24</v>
@@ -6763,10 +6763,10 @@
     </row>
     <row r="156" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
+        <v>295</v>
+      </c>
+      <c r="B156" s="2" t="s">
         <v>296</v>
-      </c>
-      <c r="B156" s="2" t="s">
-        <v>297</v>
       </c>
       <c r="C156" s="3" t="s">
         <v>9</v>
@@ -6786,10 +6786,10 @@
     </row>
     <row r="157" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
+        <v>297</v>
+      </c>
+      <c r="B157" s="77" t="s">
         <v>298</v>
-      </c>
-      <c r="B157" s="77" t="s">
-        <v>299</v>
       </c>
       <c r="C157" s="15" t="s">
         <v>40</v>
@@ -6809,7 +6809,7 @@
     </row>
     <row r="158" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B158" s="77" t="s">
         <v>76</v>
@@ -6832,10 +6832,10 @@
     </row>
     <row r="159" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
+        <v>300</v>
+      </c>
+      <c r="B159" s="8" t="s">
         <v>301</v>
-      </c>
-      <c r="B159" s="8" t="s">
-        <v>302</v>
       </c>
       <c r="C159" s="9" t="s">
         <v>26</v>
@@ -6855,10 +6855,10 @@
     </row>
     <row r="160" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
+        <v>302</v>
+      </c>
+      <c r="B160" s="14" t="s">
         <v>303</v>
-      </c>
-      <c r="B160" s="14" t="s">
-        <v>304</v>
       </c>
       <c r="C160" s="15" t="s">
         <v>40</v>
@@ -6878,10 +6878,10 @@
     </row>
     <row r="161" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B161" s="77" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C161" s="15" t="s">
         <v>40</v>
@@ -6901,10 +6901,10 @@
     </row>
     <row r="162" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
+        <v>305</v>
+      </c>
+      <c r="B162" s="77" t="s">
         <v>306</v>
-      </c>
-      <c r="B162" s="77" t="s">
-        <v>307</v>
       </c>
       <c r="C162" s="13" t="s">
         <v>35</v>
@@ -6913,7 +6913,7 @@
         <v>20</v>
       </c>
       <c r="E162" s="13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F162" s="45">
         <v>1</v>
@@ -6924,10 +6924,10 @@
     </row>
     <row r="163" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
+        <v>307</v>
+      </c>
+      <c r="B163" s="77" t="s">
         <v>308</v>
-      </c>
-      <c r="B163" s="77" t="s">
-        <v>309</v>
       </c>
       <c r="C163" s="9" t="s">
         <v>26</v>
@@ -6947,10 +6947,10 @@
     </row>
     <row r="164" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B164" s="77" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C164" s="13" t="s">
         <v>35</v>
@@ -6970,10 +6970,10 @@
     </row>
     <row r="165" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
+        <v>310</v>
+      </c>
+      <c r="B165" s="8" t="s">
         <v>311</v>
-      </c>
-      <c r="B165" s="8" t="s">
-        <v>312</v>
       </c>
       <c r="C165" s="9" t="s">
         <v>26</v>
@@ -6993,7 +6993,7 @@
     </row>
     <row r="166" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B166" s="2" t="s">
         <v>19</v>
@@ -7016,10 +7016,10 @@
     </row>
     <row r="167" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
+        <v>313</v>
+      </c>
+      <c r="B167" s="24" t="s">
         <v>314</v>
-      </c>
-      <c r="B167" s="24" t="s">
-        <v>315</v>
       </c>
       <c r="C167" s="25" t="s">
         <v>79</v>
@@ -7028,7 +7028,7 @@
         <v>30</v>
       </c>
       <c r="E167" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F167" s="53">
         <v>1</v>
@@ -7039,7 +7039,7 @@
     </row>
     <row r="168" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B168" s="14" t="s">
         <v>74</v>
@@ -7062,10 +7062,10 @@
     </row>
     <row r="169" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B169" s="77" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C169" s="9" t="s">
         <v>26</v>
@@ -7085,7 +7085,7 @@
     </row>
     <row r="170" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B170" s="2" t="s">
         <v>8</v>
@@ -7108,7 +7108,7 @@
     </row>
     <row r="171" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B171" s="14" t="s">
         <v>81</v>
@@ -7131,7 +7131,7 @@
     </row>
     <row r="172" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B172" s="14" t="s">
         <v>81</v>
@@ -7154,13 +7154,13 @@
     </row>
     <row r="173" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B173" s="36" t="s">
         <v>81</v>
       </c>
       <c r="C173" s="37" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D173" s="37">
         <v>16</v>
@@ -7177,10 +7177,10 @@
     </row>
     <row r="174" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
+        <v>321</v>
+      </c>
+      <c r="B174" s="20" t="s">
         <v>322</v>
-      </c>
-      <c r="B174" s="20" t="s">
-        <v>323</v>
       </c>
       <c r="C174" s="21" t="s">
         <v>56</v>
@@ -7200,13 +7200,13 @@
     </row>
     <row r="175" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
+        <v>323</v>
+      </c>
+      <c r="B175" s="77" t="s">
         <v>324</v>
       </c>
-      <c r="B175" s="77" t="s">
-        <v>325</v>
-      </c>
       <c r="C175" s="33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D175" s="33">
         <v>35</v>
@@ -7223,13 +7223,13 @@
     </row>
     <row r="176" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B176" s="77" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C176" s="33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D176" s="33">
         <v>16</v>
@@ -7246,13 +7246,13 @@
     </row>
     <row r="177" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
+        <v>326</v>
+      </c>
+      <c r="B177" s="77" t="s">
         <v>327</v>
       </c>
-      <c r="B177" s="77" t="s">
-        <v>328</v>
-      </c>
       <c r="C177" s="33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D177" s="33">
         <v>10</v>
@@ -7269,10 +7269,10 @@
     </row>
     <row r="178" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
+        <v>328</v>
+      </c>
+      <c r="B178" s="14" t="s">
         <v>329</v>
-      </c>
-      <c r="B178" s="14" t="s">
-        <v>330</v>
       </c>
       <c r="C178" s="15" t="s">
         <v>40</v>
@@ -7292,10 +7292,10 @@
     </row>
     <row r="179" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
+        <v>330</v>
+      </c>
+      <c r="B179" s="14" t="s">
         <v>331</v>
-      </c>
-      <c r="B179" s="14" t="s">
-        <v>332</v>
       </c>
       <c r="C179" s="15" t="s">
         <v>40</v>
@@ -7315,10 +7315,10 @@
     </row>
     <row r="180" spans="1:7" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
+        <v>332</v>
+      </c>
+      <c r="B180" s="14" t="s">
         <v>333</v>
-      </c>
-      <c r="B180" s="14" t="s">
-        <v>334</v>
       </c>
       <c r="C180" s="15" t="s">
         <v>40</v>
@@ -7338,10 +7338,10 @@
     </row>
     <row r="181" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
+        <v>334</v>
+      </c>
+      <c r="B181" s="14" t="s">
         <v>335</v>
-      </c>
-      <c r="B181" s="14" t="s">
-        <v>336</v>
       </c>
       <c r="C181" s="15" t="s">
         <v>40</v>
@@ -7361,10 +7361,10 @@
     </row>
     <row r="182" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
+        <v>336</v>
+      </c>
+      <c r="B182" s="14" t="s">
         <v>337</v>
-      </c>
-      <c r="B182" s="14" t="s">
-        <v>338</v>
       </c>
       <c r="C182" s="15" t="s">
         <v>40</v>
@@ -7384,10 +7384,10 @@
     </row>
     <row r="183" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
+        <v>338</v>
+      </c>
+      <c r="B183" s="77" t="s">
         <v>339</v>
-      </c>
-      <c r="B183" s="77" t="s">
-        <v>340</v>
       </c>
       <c r="C183" s="9" t="s">
         <v>26</v>
@@ -7407,10 +7407,10 @@
     </row>
     <row r="184" spans="1:7" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
+        <v>340</v>
+      </c>
+      <c r="B184" s="6" t="s">
         <v>341</v>
-      </c>
-      <c r="B184" s="6" t="s">
-        <v>342</v>
       </c>
       <c r="C184" s="7" t="s">
         <v>20</v>
@@ -7430,10 +7430,10 @@
     </row>
     <row r="185" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
+        <v>342</v>
+      </c>
+      <c r="B185" s="18" t="s">
         <v>343</v>
-      </c>
-      <c r="B185" s="18" t="s">
-        <v>344</v>
       </c>
       <c r="C185" s="19" t="s">
         <v>48</v>
@@ -7453,10 +7453,10 @@
     </row>
     <row r="186" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
+        <v>344</v>
+      </c>
+      <c r="B186" s="77" t="s">
         <v>345</v>
-      </c>
-      <c r="B186" s="77" t="s">
-        <v>346</v>
       </c>
       <c r="C186" s="9" t="s">
         <v>26</v>
@@ -7476,10 +7476,10 @@
     </row>
     <row r="187" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
+        <v>346</v>
+      </c>
+      <c r="B187" s="14" t="s">
         <v>347</v>
-      </c>
-      <c r="B187" s="14" t="s">
-        <v>348</v>
       </c>
       <c r="C187" s="15" t="s">
         <v>40</v>
@@ -7499,10 +7499,10 @@
     </row>
     <row r="188" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B188" s="14" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C188" s="15" t="s">
         <v>40</v>
@@ -7522,10 +7522,10 @@
     </row>
     <row r="189" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B189" s="77" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C189" s="25" t="s">
         <v>79</v>
@@ -7545,10 +7545,10 @@
     </row>
     <row r="190" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
+        <v>350</v>
+      </c>
+      <c r="B190" s="24" t="s">
         <v>351</v>
-      </c>
-      <c r="B190" s="24" t="s">
-        <v>352</v>
       </c>
       <c r="C190" s="25" t="s">
         <v>79</v>
@@ -7568,10 +7568,10 @@
     </row>
     <row r="191" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B191" s="77" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C191" s="25" t="s">
         <v>79</v>
@@ -7591,10 +7591,10 @@
     </row>
     <row r="192" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
+        <v>353</v>
+      </c>
+      <c r="B192" s="77" t="s">
         <v>354</v>
-      </c>
-      <c r="B192" s="77" t="s">
-        <v>355</v>
       </c>
       <c r="C192" s="27" t="s">
         <v>90</v>
@@ -7614,10 +7614,10 @@
     </row>
     <row r="193" spans="1:7" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
+        <v>355</v>
+      </c>
+      <c r="B193" s="14" t="s">
         <v>356</v>
-      </c>
-      <c r="B193" s="14" t="s">
-        <v>357</v>
       </c>
       <c r="C193" s="15" t="s">
         <v>40</v>
@@ -7637,7 +7637,7 @@
     </row>
     <row r="194" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B194" s="77" t="s">
         <v>65</v>
@@ -7660,10 +7660,10 @@
     </row>
     <row r="195" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
+        <v>358</v>
+      </c>
+      <c r="B195" s="16" t="s">
         <v>359</v>
-      </c>
-      <c r="B195" s="16" t="s">
-        <v>360</v>
       </c>
       <c r="C195" s="17" t="s">
         <v>43</v>
@@ -7683,10 +7683,10 @@
     </row>
     <row r="196" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
+        <v>360</v>
+      </c>
+      <c r="B196" s="77" t="s">
         <v>361</v>
-      </c>
-      <c r="B196" s="77" t="s">
-        <v>362</v>
       </c>
       <c r="C196" s="17" t="s">
         <v>43</v>
@@ -7706,10 +7706,10 @@
     </row>
     <row r="197" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
+        <v>362</v>
+      </c>
+      <c r="B197" s="77" t="s">
         <v>363</v>
-      </c>
-      <c r="B197" s="77" t="s">
-        <v>364</v>
       </c>
       <c r="C197" s="27" t="s">
         <v>90</v>
@@ -7729,10 +7729,10 @@
     </row>
     <row r="198" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B198" s="14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C198" s="15" t="s">
         <v>40</v>
@@ -7752,13 +7752,13 @@
     </row>
     <row r="199" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
+        <v>365</v>
+      </c>
+      <c r="B199" s="34" t="s">
         <v>366</v>
       </c>
-      <c r="B199" s="34" t="s">
-        <v>367</v>
-      </c>
       <c r="C199" s="35" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D199" s="35">
         <v>20</v>
@@ -7775,10 +7775,10 @@
     </row>
     <row r="200" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
+        <v>367</v>
+      </c>
+      <c r="B200" s="77" t="s">
         <v>368</v>
-      </c>
-      <c r="B200" s="77" t="s">
-        <v>369</v>
       </c>
       <c r="C200" s="23" t="s">
         <v>68</v>
@@ -7798,10 +7798,10 @@
     </row>
     <row r="201" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
+        <v>369</v>
+      </c>
+      <c r="B201" s="14" t="s">
         <v>370</v>
-      </c>
-      <c r="B201" s="14" t="s">
-        <v>371</v>
       </c>
       <c r="C201" s="15" t="s">
         <v>40</v>
@@ -7821,10 +7821,10 @@
     </row>
     <row r="202" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
+        <v>371</v>
+      </c>
+      <c r="B202" s="77" t="s">
         <v>372</v>
-      </c>
-      <c r="B202" s="77" t="s">
-        <v>373</v>
       </c>
       <c r="C202" s="15" t="s">
         <v>40</v>
@@ -7844,7 +7844,7 @@
     </row>
     <row r="203" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B203" s="6" t="s">
         <v>81</v>
@@ -7867,10 +7867,10 @@
     </row>
     <row r="204" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
+        <v>374</v>
+      </c>
+      <c r="B204" s="77" t="s">
         <v>375</v>
-      </c>
-      <c r="B204" s="77" t="s">
-        <v>376</v>
       </c>
       <c r="C204" s="15" t="s">
         <v>40</v>
@@ -7890,10 +7890,10 @@
     </row>
     <row r="205" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
+        <v>376</v>
+      </c>
+      <c r="B205" s="2" t="s">
         <v>377</v>
-      </c>
-      <c r="B205" s="2" t="s">
-        <v>378</v>
       </c>
       <c r="C205" s="3" t="s">
         <v>9</v>
@@ -7913,13 +7913,13 @@
     </row>
     <row r="206" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B206" s="77" t="s">
         <v>50</v>
       </c>
       <c r="C206" s="37" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D206" s="37">
         <v>20</v>
@@ -7936,10 +7936,10 @@
     </row>
     <row r="207" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
+        <v>379</v>
+      </c>
+      <c r="B207" s="4" t="s">
         <v>380</v>
-      </c>
-      <c r="B207" s="4" t="s">
-        <v>381</v>
       </c>
       <c r="C207" s="5" t="s">
         <v>13</v>
@@ -7959,10 +7959,10 @@
     </row>
     <row r="208" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
+        <v>381</v>
+      </c>
+      <c r="B208" s="77" t="s">
         <v>382</v>
-      </c>
-      <c r="B208" s="77" t="s">
-        <v>383</v>
       </c>
       <c r="C208" s="5" t="s">
         <v>13</v>
@@ -7982,10 +7982,10 @@
     </row>
     <row r="209" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
+        <v>383</v>
+      </c>
+      <c r="B209" s="77" t="s">
         <v>384</v>
-      </c>
-      <c r="B209" s="77" t="s">
-        <v>385</v>
       </c>
       <c r="C209" s="5" t="s">
         <v>13</v>
@@ -8005,10 +8005,10 @@
     </row>
     <row r="210" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
+        <v>385</v>
+      </c>
+      <c r="B210" s="4" t="s">
         <v>386</v>
-      </c>
-      <c r="B210" s="4" t="s">
-        <v>387</v>
       </c>
       <c r="C210" s="5" t="s">
         <v>13</v>
@@ -8028,10 +8028,10 @@
     </row>
     <row r="211" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B211" s="77" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C211" s="5" t="s">
         <v>13</v>
@@ -8051,7 +8051,7 @@
     </row>
     <row r="212" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B212" s="14" t="s">
         <v>81</v>
@@ -8074,7 +8074,7 @@
     </row>
     <row r="213" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B213" s="77" t="s">
         <v>72</v>
@@ -8097,10 +8097,10 @@
     </row>
     <row r="214" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
+        <v>390</v>
+      </c>
+      <c r="B214" s="77" t="s">
         <v>391</v>
-      </c>
-      <c r="B214" s="77" t="s">
-        <v>392</v>
       </c>
       <c r="C214" s="15" t="s">
         <v>40</v>
@@ -8109,7 +8109,7 @@
         <v>15</v>
       </c>
       <c r="E214" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F214" s="49">
         <v>0.9</v>
@@ -8120,10 +8120,10 @@
     </row>
     <row r="215" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B215" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C215" s="15" t="s">
         <v>40</v>
@@ -8143,10 +8143,10 @@
     </row>
     <row r="216" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B216" s="77" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C216" s="9" t="s">
         <v>26</v>
@@ -8166,10 +8166,10 @@
     </row>
     <row r="217" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
+        <v>394</v>
+      </c>
+      <c r="B217" s="77" t="s">
         <v>395</v>
-      </c>
-      <c r="B217" s="77" t="s">
-        <v>396</v>
       </c>
       <c r="C217" s="15" t="s">
         <v>40</v>
@@ -8192,7 +8192,7 @@
         <v>26</v>
       </c>
       <c r="B218" s="77" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C218" s="9" t="s">
         <v>26</v>
@@ -8212,10 +8212,10 @@
     </row>
     <row r="219" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
+        <v>397</v>
+      </c>
+      <c r="B219" s="77" t="s">
         <v>398</v>
-      </c>
-      <c r="B219" s="77" t="s">
-        <v>399</v>
       </c>
       <c r="C219" s="9" t="s">
         <v>26</v>
@@ -8235,10 +8235,10 @@
     </row>
     <row r="220" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B220" s="8" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C220" s="9" t="s">
         <v>26</v>
@@ -8258,10 +8258,10 @@
     </row>
     <row r="221" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
+        <v>400</v>
+      </c>
+      <c r="B221" s="77" t="s">
         <v>401</v>
-      </c>
-      <c r="B221" s="77" t="s">
-        <v>402</v>
       </c>
       <c r="C221" s="21" t="s">
         <v>56</v>
@@ -8281,10 +8281,10 @@
     </row>
     <row r="222" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B222" s="77" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C222" s="15" t="s">
         <v>40</v>
@@ -8304,10 +8304,10 @@
     </row>
     <row r="223" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
+        <v>403</v>
+      </c>
+      <c r="B223" s="77" t="s">
         <v>404</v>
-      </c>
-      <c r="B223" s="77" t="s">
-        <v>405</v>
       </c>
       <c r="C223" s="15" t="s">
         <v>40</v>
@@ -8327,10 +8327,10 @@
     </row>
     <row r="224" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
+        <v>405</v>
+      </c>
+      <c r="B224" s="26" t="s">
         <v>406</v>
-      </c>
-      <c r="B224" s="26" t="s">
-        <v>407</v>
       </c>
       <c r="C224" s="27" t="s">
         <v>90</v>
@@ -8350,10 +8350,10 @@
     </row>
     <row r="225" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
+        <v>407</v>
+      </c>
+      <c r="B225" s="14" t="s">
         <v>408</v>
-      </c>
-      <c r="B225" s="14" t="s">
-        <v>409</v>
       </c>
       <c r="C225" s="15" t="s">
         <v>40</v>
@@ -8373,7 +8373,7 @@
     </row>
     <row r="226" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B226" s="77" t="s">
         <v>23</v>
@@ -8396,10 +8396,10 @@
     </row>
     <row r="227" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
+        <v>410</v>
+      </c>
+      <c r="B227" s="14" t="s">
         <v>411</v>
-      </c>
-      <c r="B227" s="14" t="s">
-        <v>412</v>
       </c>
       <c r="C227" s="15" t="s">
         <v>40</v>
@@ -8419,10 +8419,10 @@
     </row>
     <row r="228" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B228" s="14" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C228" s="15" t="s">
         <v>40</v>
@@ -8442,10 +8442,10 @@
     </row>
     <row r="229" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
+        <v>413</v>
+      </c>
+      <c r="B229" s="14" t="s">
         <v>414</v>
-      </c>
-      <c r="B229" s="14" t="s">
-        <v>415</v>
       </c>
       <c r="C229" s="15" t="s">
         <v>40</v>
@@ -8465,10 +8465,10 @@
     </row>
     <row r="230" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
+        <v>415</v>
+      </c>
+      <c r="B230" s="8" t="s">
         <v>416</v>
-      </c>
-      <c r="B230" s="8" t="s">
-        <v>417</v>
       </c>
       <c r="C230" s="9" t="s">
         <v>26</v>
@@ -8488,10 +8488,10 @@
     </row>
     <row r="231" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
+        <v>417</v>
+      </c>
+      <c r="B231" s="14" t="s">
         <v>418</v>
-      </c>
-      <c r="B231" s="14" t="s">
-        <v>419</v>
       </c>
       <c r="C231" s="15" t="s">
         <v>40</v>
@@ -8511,10 +8511,10 @@
     </row>
     <row r="232" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
+        <v>419</v>
+      </c>
+      <c r="B232" s="8" t="s">
         <v>420</v>
-      </c>
-      <c r="B232" s="8" t="s">
-        <v>421</v>
       </c>
       <c r="C232" s="9" t="s">
         <v>26</v>
@@ -8534,10 +8534,10 @@
     </row>
     <row r="233" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
+        <v>421</v>
+      </c>
+      <c r="B233" s="77" t="s">
         <v>422</v>
-      </c>
-      <c r="B233" s="77" t="s">
-        <v>423</v>
       </c>
       <c r="C233" s="15" t="s">
         <v>40</v>
@@ -8557,10 +8557,10 @@
     </row>
     <row r="234" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
+        <v>423</v>
+      </c>
+      <c r="B234" s="12" t="s">
         <v>424</v>
-      </c>
-      <c r="B234" s="12" t="s">
-        <v>425</v>
       </c>
       <c r="C234" s="13" t="s">
         <v>35</v>
@@ -8580,10 +8580,10 @@
     </row>
     <row r="235" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B235" s="77" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C235" s="13" t="s">
         <v>35</v>
@@ -8592,7 +8592,7 @@
         <v>5</v>
       </c>
       <c r="E235" s="13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F235" s="45">
         <v>1</v>
@@ -8603,10 +8603,10 @@
     </row>
     <row r="236" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
+        <v>426</v>
+      </c>
+      <c r="B236" s="14" t="s">
         <v>427</v>
-      </c>
-      <c r="B236" s="14" t="s">
-        <v>428</v>
       </c>
       <c r="C236" s="15" t="s">
         <v>40</v>
@@ -8626,7 +8626,7 @@
     </row>
     <row r="237" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B237" s="77" t="s">
         <v>50</v>
@@ -8649,7 +8649,7 @@
     </row>
     <row r="238" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B238" s="77" t="s">
         <v>65</v>
@@ -8672,10 +8672,10 @@
     </row>
     <row r="239" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B239" s="77" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C239" s="13" t="s">
         <v>35</v>
@@ -8695,7 +8695,7 @@
     </row>
     <row r="240" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B240" s="10" t="s">
         <v>81</v>
@@ -8718,10 +8718,10 @@
     </row>
     <row r="241" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B241" s="77" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C241" s="11" t="s">
         <v>33</v>
@@ -8741,10 +8741,10 @@
     </row>
     <row r="242" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
+        <v>433</v>
+      </c>
+      <c r="B242" s="77" t="s">
         <v>434</v>
-      </c>
-      <c r="B242" s="77" t="s">
-        <v>435</v>
       </c>
       <c r="C242" s="9" t="s">
         <v>26</v>
@@ -8764,7 +8764,7 @@
     </row>
     <row r="243" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B243" s="77" t="s">
         <v>65</v>
@@ -8787,10 +8787,10 @@
     </row>
     <row r="244" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B244" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C244" s="11" t="s">
         <v>33</v>
@@ -8810,10 +8810,10 @@
     </row>
     <row r="245" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
+        <v>437</v>
+      </c>
+      <c r="B245" s="22" t="s">
         <v>438</v>
-      </c>
-      <c r="B245" s="22" t="s">
-        <v>439</v>
       </c>
       <c r="C245" s="23" t="s">
         <v>68</v>
@@ -8833,10 +8833,10 @@
     </row>
     <row r="246" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
+        <v>439</v>
+      </c>
+      <c r="B246" s="77" t="s">
         <v>440</v>
-      </c>
-      <c r="B246" s="77" t="s">
-        <v>441</v>
       </c>
       <c r="C246" s="15" t="s">
         <v>40</v>
@@ -8856,7 +8856,7 @@
     </row>
     <row r="247" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B247" s="24" t="s">
         <v>63</v>
@@ -8879,10 +8879,10 @@
     </row>
     <row r="248" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B248" s="77" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C248" s="25" t="s">
         <v>79</v>
@@ -8902,10 +8902,10 @@
     </row>
     <row r="249" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
+        <v>443</v>
+      </c>
+      <c r="B249" s="10" t="s">
         <v>444</v>
-      </c>
-      <c r="B249" s="10" t="s">
-        <v>445</v>
       </c>
       <c r="C249" s="11" t="s">
         <v>33</v>
@@ -8925,10 +8925,10 @@
     </row>
     <row r="250" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B250" s="77" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C250" s="15" t="s">
         <v>40</v>
@@ -8948,7 +8948,7 @@
     </row>
     <row r="251" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B251" s="14" t="s">
         <v>81</v>
@@ -8971,10 +8971,10 @@
     </row>
     <row r="252" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
+        <v>447</v>
+      </c>
+      <c r="B252" s="77" t="s">
         <v>448</v>
-      </c>
-      <c r="B252" s="77" t="s">
-        <v>449</v>
       </c>
       <c r="C252" s="15" t="s">
         <v>40</v>
@@ -8994,10 +8994,10 @@
     </row>
     <row r="253" spans="1:7" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
+        <v>449</v>
+      </c>
+      <c r="B253" s="14" t="s">
         <v>450</v>
-      </c>
-      <c r="B253" s="14" t="s">
-        <v>451</v>
       </c>
       <c r="C253" s="15" t="s">
         <v>40</v>
@@ -9017,10 +9017,10 @@
     </row>
     <row r="254" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B254" s="12" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C254" s="13" t="s">
         <v>35</v>
@@ -9040,10 +9040,10 @@
     </row>
     <row r="255" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B255" s="77" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C255" s="15" t="s">
         <v>40</v>
@@ -9063,10 +9063,10 @@
     </row>
     <row r="256" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B256" s="77" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C256" s="17" t="s">
         <v>43</v>
@@ -9086,7 +9086,7 @@
     </row>
     <row r="257" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B257" s="16" t="s">
         <v>19</v>
@@ -9109,10 +9109,10 @@
     </row>
     <row r="258" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B258" s="77" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C258" s="15" t="s">
         <v>40</v>
@@ -9132,10 +9132,10 @@
     </row>
     <row r="259" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B259" s="77" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C259" s="19" t="s">
         <v>48</v>
@@ -9144,7 +9144,7 @@
         <v>5</v>
       </c>
       <c r="E259" s="19" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F259" s="50">
         <v>0.3</v>
@@ -9155,13 +9155,13 @@
     </row>
     <row r="260" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B260" s="28" t="s">
         <v>19</v>
       </c>
       <c r="C260" s="29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D260" s="29">
         <v>20</v>
@@ -9178,13 +9178,13 @@
     </row>
     <row r="261" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B261" s="77" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C261" s="37" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D261" s="37">
         <v>24</v>
@@ -9201,13 +9201,13 @@
     </row>
     <row r="262" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B262" s="77" t="s">
         <v>32</v>
       </c>
       <c r="C262" s="37" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D262" s="37">
         <v>5</v>
@@ -9224,10 +9224,10 @@
     </row>
     <row r="263" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B263" s="77" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C263" s="15" t="s">
         <v>40</v>
@@ -9247,10 +9247,10 @@
     </row>
     <row r="264" spans="1:7" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
+        <v>461</v>
+      </c>
+      <c r="B264" s="14" t="s">
         <v>462</v>
-      </c>
-      <c r="B264" s="14" t="s">
-        <v>463</v>
       </c>
       <c r="C264" s="15" t="s">
         <v>40</v>
@@ -9270,10 +9270,10 @@
     </row>
     <row r="265" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
+        <v>463</v>
+      </c>
+      <c r="B265" s="77" t="s">
         <v>464</v>
-      </c>
-      <c r="B265" s="77" t="s">
-        <v>465</v>
       </c>
       <c r="C265" s="9" t="s">
         <v>26</v>
@@ -9293,10 +9293,10 @@
     </row>
     <row r="266" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
+        <v>465</v>
+      </c>
+      <c r="B266" s="14" t="s">
         <v>466</v>
-      </c>
-      <c r="B266" s="14" t="s">
-        <v>467</v>
       </c>
       <c r="C266" s="15" t="s">
         <v>40</v>
@@ -9316,10 +9316,10 @@
     </row>
     <row r="267" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
+        <v>467</v>
+      </c>
+      <c r="B267" s="6" t="s">
         <v>468</v>
-      </c>
-      <c r="B267" s="6" t="s">
-        <v>469</v>
       </c>
       <c r="C267" s="7" t="s">
         <v>20</v>
@@ -9339,10 +9339,10 @@
     </row>
     <row r="268" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
+        <v>469</v>
+      </c>
+      <c r="B268" s="12" t="s">
         <v>470</v>
-      </c>
-      <c r="B268" s="12" t="s">
-        <v>471</v>
       </c>
       <c r="C268" s="13" t="s">
         <v>35</v>
@@ -9362,10 +9362,10 @@
     </row>
     <row r="269" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B269" s="14" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C269" s="15" t="s">
         <v>40</v>
@@ -9385,7 +9385,7 @@
     </row>
     <row r="270" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B270" s="14" t="s">
         <v>81</v>
@@ -9408,7 +9408,7 @@
     </row>
     <row r="271" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B271" s="77" t="s">
         <v>23</v>
@@ -9431,10 +9431,10 @@
     </row>
     <row r="272" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B272" s="77" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C272" s="3" t="s">
         <v>9</v>
@@ -9454,10 +9454,10 @@
     </row>
     <row r="273" spans="1:7" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
+        <v>475</v>
+      </c>
+      <c r="B273" s="14" t="s">
         <v>476</v>
-      </c>
-      <c r="B273" s="14" t="s">
-        <v>477</v>
       </c>
       <c r="C273" s="15" t="s">
         <v>40</v>
@@ -9477,10 +9477,10 @@
     </row>
     <row r="274" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
+        <v>477</v>
+      </c>
+      <c r="B274" s="77" t="s">
         <v>478</v>
-      </c>
-      <c r="B274" s="77" t="s">
-        <v>479</v>
       </c>
       <c r="C274" s="5" t="s">
         <v>13</v>
@@ -9500,10 +9500,10 @@
     </row>
     <row r="275" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B275" s="77" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C275" s="5" t="s">
         <v>13</v>
@@ -9523,10 +9523,10 @@
     </row>
     <row r="276" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
+        <v>480</v>
+      </c>
+      <c r="B276" s="77" t="s">
         <v>481</v>
-      </c>
-      <c r="B276" s="77" t="s">
-        <v>482</v>
       </c>
       <c r="C276" s="15" t="s">
         <v>40</v>
@@ -9546,10 +9546,10 @@
     </row>
     <row r="277" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
+        <v>482</v>
+      </c>
+      <c r="B277" s="77" t="s">
         <v>483</v>
-      </c>
-      <c r="B277" s="77" t="s">
-        <v>484</v>
       </c>
       <c r="C277" s="5" t="s">
         <v>13</v>
@@ -9569,10 +9569,10 @@
     </row>
     <row r="278" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B278" s="77" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C278" s="15" t="s">
         <v>40</v>
@@ -9592,10 +9592,10 @@
     </row>
     <row r="279" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
+        <v>485</v>
+      </c>
+      <c r="B279" s="20" t="s">
         <v>486</v>
-      </c>
-      <c r="B279" s="20" t="s">
-        <v>487</v>
       </c>
       <c r="C279" s="21" t="s">
         <v>56</v>
@@ -9615,10 +9615,10 @@
     </row>
     <row r="280" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
+        <v>487</v>
+      </c>
+      <c r="B280" s="77" t="s">
         <v>488</v>
-      </c>
-      <c r="B280" s="77" t="s">
-        <v>489</v>
       </c>
       <c r="C280" s="15" t="s">
         <v>40</v>
@@ -9638,10 +9638,10 @@
     </row>
     <row r="281" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B281" s="14" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C281" s="15" t="s">
         <v>40</v>
@@ -9661,10 +9661,10 @@
     </row>
     <row r="282" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
+        <v>490</v>
+      </c>
+      <c r="B282" s="2" t="s">
         <v>491</v>
-      </c>
-      <c r="B282" s="2" t="s">
-        <v>492</v>
       </c>
       <c r="C282" s="3" t="s">
         <v>9</v>
@@ -9684,10 +9684,10 @@
     </row>
     <row r="283" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
+        <v>492</v>
+      </c>
+      <c r="B283" s="14" t="s">
         <v>493</v>
-      </c>
-      <c r="B283" s="14" t="s">
-        <v>494</v>
       </c>
       <c r="C283" s="15" t="s">
         <v>40</v>
@@ -9696,7 +9696,7 @@
         <v>20</v>
       </c>
       <c r="E283" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F283" s="49">
         <v>1</v>
@@ -9707,13 +9707,13 @@
     </row>
     <row r="284" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B284" s="77" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C284" s="29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D284" s="29">
         <v>20</v>
@@ -9730,13 +9730,13 @@
     </row>
     <row r="285" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B285" s="36" t="s">
         <v>74</v>
       </c>
       <c r="C285" s="37" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D285" s="37">
         <v>10</v>
@@ -9753,7 +9753,7 @@
     </row>
     <row r="286" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B286" s="77" t="s">
         <v>50</v>
@@ -9776,10 +9776,10 @@
     </row>
     <row r="287" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
+        <v>497</v>
+      </c>
+      <c r="B287" s="24" t="s">
         <v>498</v>
-      </c>
-      <c r="B287" s="24" t="s">
-        <v>499</v>
       </c>
       <c r="C287" s="25" t="s">
         <v>79</v>
@@ -9799,7 +9799,7 @@
     </row>
     <row r="288" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B288" s="14" t="s">
         <v>81</v>
@@ -9822,10 +9822,10 @@
     </row>
     <row r="289" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
+        <v>500</v>
+      </c>
+      <c r="B289" s="77" t="s">
         <v>501</v>
-      </c>
-      <c r="B289" s="77" t="s">
-        <v>502</v>
       </c>
       <c r="C289" s="17" t="s">
         <v>43</v>
@@ -9845,10 +9845,10 @@
     </row>
     <row r="290" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
+        <v>502</v>
+      </c>
+      <c r="B290" s="14" t="s">
         <v>503</v>
-      </c>
-      <c r="B290" s="14" t="s">
-        <v>504</v>
       </c>
       <c r="C290" s="15" t="s">
         <v>40</v>
@@ -9868,10 +9868,10 @@
     </row>
     <row r="291" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B291" s="77" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C291" s="3" t="s">
         <v>9</v>
@@ -9891,13 +9891,13 @@
     </row>
     <row r="292" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
+        <v>505</v>
+      </c>
+      <c r="B292" s="77" t="s">
         <v>506</v>
       </c>
-      <c r="B292" s="77" t="s">
-        <v>507</v>
-      </c>
       <c r="C292" s="33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D292" s="33">
         <v>25</v>
@@ -9914,10 +9914,10 @@
     </row>
     <row r="293" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
+        <v>507</v>
+      </c>
+      <c r="B293" s="14" t="s">
         <v>508</v>
-      </c>
-      <c r="B293" s="14" t="s">
-        <v>509</v>
       </c>
       <c r="C293" s="15" t="s">
         <v>40</v>
@@ -9937,10 +9937,10 @@
     </row>
     <row r="294" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
+        <v>509</v>
+      </c>
+      <c r="B294" s="14" t="s">
         <v>510</v>
-      </c>
-      <c r="B294" s="14" t="s">
-        <v>511</v>
       </c>
       <c r="C294" s="15" t="s">
         <v>40</v>
@@ -9960,7 +9960,7 @@
     </row>
     <row r="295" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B295" s="14" t="s">
         <v>81</v>
@@ -9983,13 +9983,13 @@
     </row>
     <row r="296" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B296" s="77" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C296" s="37" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D296" s="37">
         <v>5</v>
@@ -10006,10 +10006,10 @@
     </row>
     <row r="297" spans="1:7" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
+        <v>513</v>
+      </c>
+      <c r="B297" s="77" t="s">
         <v>514</v>
-      </c>
-      <c r="B297" s="77" t="s">
-        <v>515</v>
       </c>
       <c r="C297" s="38" t="s">
         <v>40</v>
@@ -10029,10 +10029,10 @@
     </row>
     <row r="298" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B298" s="77" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C298" s="3" t="s">
         <v>9</v>
@@ -10052,10 +10052,10 @@
     </row>
     <row r="299" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
+        <v>516</v>
+      </c>
+      <c r="B299" s="12" t="s">
         <v>517</v>
-      </c>
-      <c r="B299" s="12" t="s">
-        <v>518</v>
       </c>
       <c r="C299" s="13" t="s">
         <v>35</v>
@@ -10075,10 +10075,10 @@
     </row>
     <row r="300" spans="1:7" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
+        <v>518</v>
+      </c>
+      <c r="B300" s="14" t="s">
         <v>519</v>
-      </c>
-      <c r="B300" s="14" t="s">
-        <v>520</v>
       </c>
       <c r="C300" s="15" t="s">
         <v>40</v>
@@ -10098,10 +10098,10 @@
     </row>
     <row r="301" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
+        <v>520</v>
+      </c>
+      <c r="B301" s="22" t="s">
         <v>521</v>
-      </c>
-      <c r="B301" s="22" t="s">
-        <v>522</v>
       </c>
       <c r="C301" s="23" t="s">
         <v>68</v>
@@ -10121,10 +10121,10 @@
     </row>
     <row r="302" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
+        <v>522</v>
+      </c>
+      <c r="B302" s="77" t="s">
         <v>523</v>
-      </c>
-      <c r="B302" s="77" t="s">
-        <v>524</v>
       </c>
       <c r="C302" s="21" t="s">
         <v>56</v>
@@ -10133,7 +10133,7 @@
         <v>16</v>
       </c>
       <c r="E302" s="21" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="F302" s="51">
         <v>1</v>
@@ -10144,10 +10144,10 @@
     </row>
     <row r="303" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
+        <v>525</v>
+      </c>
+      <c r="B303" s="77" t="s">
         <v>526</v>
-      </c>
-      <c r="B303" s="77" t="s">
-        <v>527</v>
       </c>
       <c r="C303" s="13" t="s">
         <v>35</v>
@@ -10167,10 +10167,10 @@
     </row>
     <row r="304" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B304" s="77" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C304" s="15" t="s">
         <v>40</v>
@@ -10190,10 +10190,10 @@
     </row>
     <row r="305" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
+        <v>528</v>
+      </c>
+      <c r="B305" s="77" t="s">
         <v>529</v>
-      </c>
-      <c r="B305" s="77" t="s">
-        <v>530</v>
       </c>
       <c r="C305" s="27" t="s">
         <v>90</v>
@@ -10213,10 +10213,10 @@
     </row>
     <row r="306" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
+        <v>530</v>
+      </c>
+      <c r="B306" s="14" t="s">
         <v>531</v>
-      </c>
-      <c r="B306" s="14" t="s">
-        <v>532</v>
       </c>
       <c r="C306" s="15" t="s">
         <v>40</v>
@@ -10236,10 +10236,10 @@
     </row>
     <row r="307" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B307" s="77" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C307" s="15" t="s">
         <v>40</v>
@@ -10259,10 +10259,10 @@
     </row>
     <row r="308" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B308" s="77" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C308" s="15" t="s">
         <v>40</v>
@@ -10282,10 +10282,10 @@
     </row>
     <row r="309" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
+        <v>534</v>
+      </c>
+      <c r="B309" s="77" t="s">
         <v>535</v>
-      </c>
-      <c r="B309" s="77" t="s">
-        <v>536</v>
       </c>
       <c r="C309" s="15" t="s">
         <v>40</v>
@@ -10305,7 +10305,7 @@
     </row>
     <row r="310" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B310" s="14" t="s">
         <v>19</v>
@@ -10328,10 +10328,10 @@
     </row>
     <row r="311" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
+        <v>537</v>
+      </c>
+      <c r="B311" s="77" t="s">
         <v>538</v>
-      </c>
-      <c r="B311" s="77" t="s">
-        <v>539</v>
       </c>
       <c r="C311" s="15" t="s">
         <v>40</v>
@@ -10351,10 +10351,10 @@
     </row>
     <row r="312" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B312" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C312" s="3" t="s">
         <v>9</v>
@@ -10374,7 +10374,7 @@
     </row>
     <row r="313" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B313" s="14" t="s">
         <v>81</v>
@@ -10397,13 +10397,13 @@
     </row>
     <row r="314" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
+        <v>541</v>
+      </c>
+      <c r="B314" s="77" t="s">
         <v>542</v>
       </c>
-      <c r="B314" s="77" t="s">
-        <v>543</v>
-      </c>
       <c r="C314" s="37" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D314" s="37">
         <v>3</v>
@@ -10420,10 +10420,10 @@
     </row>
     <row r="315" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B315" s="77" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C315" s="15" t="s">
         <v>40</v>
@@ -10443,10 +10443,10 @@
     </row>
     <row r="316" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B316" s="14" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C316" s="15" t="s">
         <v>40</v>
@@ -10466,10 +10466,10 @@
     </row>
     <row r="317" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
+        <v>545</v>
+      </c>
+      <c r="B317" s="20" t="s">
         <v>546</v>
-      </c>
-      <c r="B317" s="20" t="s">
-        <v>547</v>
       </c>
       <c r="C317" s="21" t="s">
         <v>56</v>
@@ -10489,10 +10489,10 @@
     </row>
     <row r="318" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
+        <v>547</v>
+      </c>
+      <c r="B318" s="77" t="s">
         <v>548</v>
-      </c>
-      <c r="B318" s="77" t="s">
-        <v>549</v>
       </c>
       <c r="C318" s="15" t="s">
         <v>40</v>
@@ -10512,10 +10512,10 @@
     </row>
     <row r="319" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
+        <v>549</v>
+      </c>
+      <c r="B319" s="8" t="s">
         <v>550</v>
-      </c>
-      <c r="B319" s="8" t="s">
-        <v>551</v>
       </c>
       <c r="C319" s="9" t="s">
         <v>26</v>
@@ -10535,10 +10535,10 @@
     </row>
     <row r="320" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
+        <v>551</v>
+      </c>
+      <c r="B320" s="77" t="s">
         <v>552</v>
-      </c>
-      <c r="B320" s="77" t="s">
-        <v>553</v>
       </c>
       <c r="C320" s="21" t="s">
         <v>56</v>
@@ -10558,10 +10558,10 @@
     </row>
     <row r="321" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B321" s="14" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C321" s="15" t="s">
         <v>40</v>
@@ -10581,13 +10581,13 @@
     </row>
     <row r="322" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
+        <v>554</v>
+      </c>
+      <c r="B322" s="28" t="s">
         <v>555</v>
       </c>
-      <c r="B322" s="28" t="s">
-        <v>556</v>
-      </c>
       <c r="C322" s="29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D322" s="29">
         <v>16</v>
@@ -10604,13 +10604,13 @@
     </row>
     <row r="323" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B323" s="77" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C323" s="29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D323" s="29">
         <v>16</v>
@@ -10627,13 +10627,13 @@
     </row>
     <row r="324" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
+        <v>557</v>
+      </c>
+      <c r="B324" s="77" t="s">
         <v>558</v>
       </c>
-      <c r="B324" s="77" t="s">
-        <v>559</v>
-      </c>
       <c r="C324" s="29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D324" s="29">
         <v>24</v>
@@ -10650,13 +10650,13 @@
     </row>
     <row r="325" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B325" s="77" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C325" s="29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D325" s="29">
         <v>15</v>
@@ -10673,13 +10673,13 @@
     </row>
     <row r="326" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B326" s="77" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C326" s="29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D326" s="29">
         <v>30</v>
@@ -10696,10 +10696,10 @@
     </row>
     <row r="327" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
+        <v>561</v>
+      </c>
+      <c r="B327" s="77" t="s">
         <v>562</v>
-      </c>
-      <c r="B327" s="77" t="s">
-        <v>563</v>
       </c>
       <c r="C327" s="15" t="s">
         <v>40</v>
@@ -10719,10 +10719,10 @@
     </row>
     <row r="328" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
+        <v>563</v>
+      </c>
+      <c r="B328" s="77" t="s">
         <v>564</v>
-      </c>
-      <c r="B328" s="77" t="s">
-        <v>565</v>
       </c>
       <c r="C328" s="21" t="s">
         <v>56</v>
@@ -10742,10 +10742,10 @@
     </row>
     <row r="329" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
+        <v>565</v>
+      </c>
+      <c r="B329" s="77" t="s">
         <v>566</v>
-      </c>
-      <c r="B329" s="77" t="s">
-        <v>567</v>
       </c>
       <c r="C329" s="5" t="s">
         <v>13</v>
@@ -10765,10 +10765,10 @@
     </row>
     <row r="330" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
+        <v>567</v>
+      </c>
+      <c r="B330" s="14" t="s">
         <v>568</v>
-      </c>
-      <c r="B330" s="14" t="s">
-        <v>569</v>
       </c>
       <c r="C330" s="15" t="s">
         <v>40</v>
@@ -10788,10 +10788,10 @@
     </row>
     <row r="331" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
+        <v>569</v>
+      </c>
+      <c r="B331" s="14" t="s">
         <v>570</v>
-      </c>
-      <c r="B331" s="14" t="s">
-        <v>571</v>
       </c>
       <c r="C331" s="15" t="s">
         <v>40</v>
@@ -10811,10 +10811,10 @@
     </row>
     <row r="332" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
+        <v>571</v>
+      </c>
+      <c r="B332" s="8" t="s">
         <v>572</v>
-      </c>
-      <c r="B332" s="8" t="s">
-        <v>573</v>
       </c>
       <c r="C332" s="9" t="s">
         <v>26</v>
@@ -10834,10 +10834,10 @@
     </row>
     <row r="333" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
+        <v>573</v>
+      </c>
+      <c r="B333" s="77" t="s">
         <v>574</v>
-      </c>
-      <c r="B333" s="77" t="s">
-        <v>575</v>
       </c>
       <c r="C333" s="13" t="s">
         <v>35</v>
@@ -10857,13 +10857,13 @@
     </row>
     <row r="334" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
+        <v>575</v>
+      </c>
+      <c r="B334" s="36" t="s">
         <v>576</v>
       </c>
-      <c r="B334" s="36" t="s">
-        <v>577</v>
-      </c>
       <c r="C334" s="37" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D334" s="37">
         <v>20</v>
@@ -10880,13 +10880,13 @@
     </row>
     <row r="335" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
+        <v>577</v>
+      </c>
+      <c r="B335" s="34" t="s">
         <v>578</v>
       </c>
-      <c r="B335" s="34" t="s">
-        <v>579</v>
-      </c>
       <c r="C335" s="35" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D335" s="35">
         <v>20</v>
@@ -10903,10 +10903,10 @@
     </row>
     <row r="336" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
+        <v>579</v>
+      </c>
+      <c r="B336" s="14" t="s">
         <v>580</v>
-      </c>
-      <c r="B336" s="14" t="s">
-        <v>581</v>
       </c>
       <c r="C336" s="15" t="s">
         <v>40</v>
@@ -10926,7 +10926,7 @@
     </row>
     <row r="337" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B337" s="14" t="s">
         <v>81</v>
@@ -10949,7 +10949,7 @@
     </row>
     <row r="338" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B338" s="2" t="s">
         <v>81</v>
@@ -10972,10 +10972,10 @@
     </row>
     <row r="339" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
+        <v>583</v>
+      </c>
+      <c r="B339" s="12" t="s">
         <v>584</v>
-      </c>
-      <c r="B339" s="12" t="s">
-        <v>585</v>
       </c>
       <c r="C339" s="13" t="s">
         <v>35</v>
@@ -10995,13 +10995,13 @@
     </row>
     <row r="340" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B340" s="28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C340" s="29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D340" s="29">
         <v>15</v>
@@ -11018,7 +11018,7 @@
     </row>
     <row r="341" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B341" s="26" t="s">
         <v>81</v>
@@ -11041,10 +11041,10 @@
     </row>
     <row r="342" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B342" s="77" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C342" s="27" t="s">
         <v>90</v>
@@ -11064,10 +11064,10 @@
     </row>
     <row r="343" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
+        <v>588</v>
+      </c>
+      <c r="B343" s="26" t="s">
         <v>589</v>
-      </c>
-      <c r="B343" s="26" t="s">
-        <v>590</v>
       </c>
       <c r="C343" s="27" t="s">
         <v>90</v>
@@ -11087,10 +11087,10 @@
     </row>
     <row r="344" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
+        <v>590</v>
+      </c>
+      <c r="B344" s="77" t="s">
         <v>591</v>
-      </c>
-      <c r="B344" s="77" t="s">
-        <v>592</v>
       </c>
       <c r="C344" s="27" t="s">
         <v>90</v>
@@ -11110,7 +11110,7 @@
     </row>
     <row r="345" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B345" s="26" t="s">
         <v>81</v>
@@ -11133,10 +11133,10 @@
     </row>
     <row r="346" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
+        <v>593</v>
+      </c>
+      <c r="B346" s="14" t="s">
         <v>594</v>
-      </c>
-      <c r="B346" s="14" t="s">
-        <v>595</v>
       </c>
       <c r="C346" s="15" t="s">
         <v>40</v>
@@ -11156,10 +11156,10 @@
     </row>
     <row r="347" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
+        <v>595</v>
+      </c>
+      <c r="B347" s="26" t="s">
         <v>596</v>
-      </c>
-      <c r="B347" s="26" t="s">
-        <v>597</v>
       </c>
       <c r="C347" s="27" t="s">
         <v>90</v>
@@ -11179,10 +11179,10 @@
     </row>
     <row r="348" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
+        <v>597</v>
+      </c>
+      <c r="B348" s="14" t="s">
         <v>598</v>
-      </c>
-      <c r="B348" s="14" t="s">
-        <v>599</v>
       </c>
       <c r="C348" s="15" t="s">
         <v>40</v>
@@ -11202,10 +11202,10 @@
     </row>
     <row r="349" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
+        <v>599</v>
+      </c>
+      <c r="B349" s="22" t="s">
         <v>600</v>
-      </c>
-      <c r="B349" s="22" t="s">
-        <v>601</v>
       </c>
       <c r="C349" s="23" t="s">
         <v>68</v>
@@ -11225,7 +11225,7 @@
     </row>
     <row r="350" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B350" s="6" t="s">
         <v>81</v>
@@ -11248,10 +11248,10 @@
     </row>
     <row r="351" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
+        <v>602</v>
+      </c>
+      <c r="B351" s="14" t="s">
         <v>603</v>
-      </c>
-      <c r="B351" s="14" t="s">
-        <v>604</v>
       </c>
       <c r="C351" s="15" t="s">
         <v>40</v>
@@ -11271,10 +11271,10 @@
     </row>
     <row r="352" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B352" s="77" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C352" s="27" t="s">
         <v>90</v>
@@ -11294,7 +11294,7 @@
     </row>
     <row r="353" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B353" s="14" t="s">
         <v>63</v>
@@ -11317,10 +11317,10 @@
     </row>
     <row r="354" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
+        <v>606</v>
+      </c>
+      <c r="B354" s="77" t="s">
         <v>607</v>
-      </c>
-      <c r="B354" s="77" t="s">
-        <v>608</v>
       </c>
       <c r="C354" s="15" t="s">
         <v>40</v>
@@ -11340,13 +11340,13 @@
     </row>
     <row r="355" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B355" s="77" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C355" s="75" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D355" s="75">
         <v>5</v>

</xml_diff>